<commit_message>
original raw data file
</commit_message>
<xml_diff>
--- a/Running_Log.xlsx
+++ b/Running_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlexDolwick/dolwick_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC312D42-0A7C-2B4E-B088-E7CF9B743538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E879143-9263-0B4C-AD91-F488E40DDE79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="460" windowWidth="25680" windowHeight="15920" xr2:uid="{4B2E00A5-7125-EC4E-9EAD-C4CEE86B127A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3655" uniqueCount="3105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3657" uniqueCount="3106">
   <si>
     <t>Date</t>
   </si>
@@ -9346,6 +9346,9 @@
   </si>
   <si>
     <t>46:36</t>
+  </si>
+  <si>
+    <t>2019-12-13</t>
   </si>
 </sst>
 </file>
@@ -9719,10 +9722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BECE25-7878-7543-A5E4-1B4438F2AAC2}">
-  <dimension ref="A1:C2388"/>
+  <dimension ref="A1:C2389"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2373" workbookViewId="0">
-      <selection activeCell="C2391" sqref="C2391"/>
+      <selection activeCell="C2390" sqref="C2390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34299,6 +34302,17 @@
         <v>3104</v>
       </c>
     </row>
+    <row r="2389" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2389" s="2" t="s">
+        <v>3105</v>
+      </c>
+      <c r="B2389" s="1">
+        <v>6.55</v>
+      </c>
+      <c r="C2389" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
final 2010s update to running log
</commit_message>
<xml_diff>
--- a/Running_Log.xlsx
+++ b/Running_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlexDolwick/dolwick_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC6B153-5623-3941-ACD2-69F152CCEE18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1486B113-970A-1F42-B11D-CA23CAFC1128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="460" windowWidth="25680" windowHeight="15920" xr2:uid="{4B2E00A5-7125-EC4E-9EAD-C4CEE86B127A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3668" uniqueCount="3113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3670" uniqueCount="3115">
   <si>
     <t>Date</t>
   </si>
@@ -9370,6 +9370,12 @@
   </si>
   <si>
     <t>35:19</t>
+  </si>
+  <si>
+    <t>2019-12-24</t>
+  </si>
+  <si>
+    <t>40:17</t>
   </si>
 </sst>
 </file>
@@ -9743,10 +9749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BECE25-7878-7543-A5E4-1B4438F2AAC2}">
-  <dimension ref="A1:C2395"/>
+  <dimension ref="A1:C2396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2373" workbookViewId="0">
-      <selection activeCell="C2395" sqref="C2395"/>
+    <sheetView tabSelected="1" topLeftCell="A2379" workbookViewId="0">
+      <selection activeCell="A2397" sqref="A2397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34397,6 +34403,17 @@
         <v>3112</v>
       </c>
     </row>
+    <row r="2396" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2396" s="2" t="s">
+        <v>3113</v>
+      </c>
+      <c r="B2396" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2396" s="2" t="s">
+        <v>3114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
2020 update, fixed an errant data point
</commit_message>
<xml_diff>
--- a/Running_Log.xlsx
+++ b/Running_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlexDolwick/dolwick_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF21FD32-38AD-FF45-8E84-8A5234502340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3371DA8E-B468-594D-83A1-608F1A8FAD7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="460" windowWidth="25680" windowHeight="15920" xr2:uid="{4B2E00A5-7125-EC4E-9EAD-C4CEE86B127A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3697" uniqueCount="3136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3697" uniqueCount="3137">
   <si>
     <t>Date</t>
   </si>
@@ -9439,6 +9439,9 @@
   </si>
   <si>
     <t>48:25</t>
+  </si>
+  <si>
+    <t>1:09:59</t>
   </si>
 </sst>
 </file>
@@ -9814,8 +9817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BECE25-7878-7543-A5E4-1B4438F2AAC2}">
   <dimension ref="A1:C2410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2382" workbookViewId="0">
-      <selection activeCell="A2411" sqref="A2411"/>
+    <sheetView tabSelected="1" topLeftCell="A1263" workbookViewId="0">
+      <selection activeCell="F1276" sqref="F1276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23202,7 +23205,7 @@
         <v>9.15</v>
       </c>
       <c r="C1272" s="2" t="s">
-        <v>756</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="1273" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
4apr2020 update and df edits
</commit_message>
<xml_diff>
--- a/Running_Log.xlsx
+++ b/Running_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlexDolwick/dolwick_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349F004C-EE31-364C-AEEB-F9B3E0FEE480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA465090-8CBE-154C-96DA-B40F704CF4C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25680" windowHeight="15920" xr2:uid="{4B2E00A5-7125-EC4E-9EAD-C4CEE86B127A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3815" uniqueCount="3235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3822" uniqueCount="3241">
   <si>
     <t>Date</t>
   </si>
@@ -9738,6 +9738,24 @@
   </si>
   <si>
     <t>2020-03-31</t>
+  </si>
+  <si>
+    <t>2020-04-01</t>
+  </si>
+  <si>
+    <t>49:48</t>
+  </si>
+  <si>
+    <t>2020-04-02</t>
+  </si>
+  <si>
+    <t>2020-04-03</t>
+  </si>
+  <si>
+    <t>2020-04-04</t>
+  </si>
+  <si>
+    <t>1:47:10</t>
   </si>
 </sst>
 </file>
@@ -10111,10 +10129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BECE25-7878-7543-A5E4-1B4438F2AAC2}">
-  <dimension ref="A1:C2472"/>
+  <dimension ref="A1:C2476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2446" workbookViewId="0">
-      <selection activeCell="C2473" sqref="C2473"/>
+    <sheetView tabSelected="1" topLeftCell="A2452" workbookViewId="0">
+      <selection activeCell="D2479" sqref="D2479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35591,6 +35609,47 @@
         <v>1787</v>
       </c>
     </row>
+    <row r="2473" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2473" s="2" t="s">
+        <v>3235</v>
+      </c>
+      <c r="B2473" s="1">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="C2473" s="2" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="2474" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2474" s="2" t="s">
+        <v>3237</v>
+      </c>
+      <c r="B2474" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2475" s="2" t="s">
+        <v>3238</v>
+      </c>
+      <c r="B2475" s="1">
+        <v>7.14</v>
+      </c>
+      <c r="C2475" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2476" s="2" t="s">
+        <v>3239</v>
+      </c>
+      <c r="B2476" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="C2476" s="2" t="s">
+        <v>3240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
added 2021 to figures, incl pace_distance scatterplot
</commit_message>
<xml_diff>
--- a/Running_Log.xlsx
+++ b/Running_Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlexDolwick/dolwick_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE7A8E9-D0E9-F540-95B6-707923378F25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE7FBFB-5C83-A345-A90C-D8AECC996029}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25680" windowHeight="15920" xr2:uid="{4B2E00A5-7125-EC4E-9EAD-C4CEE86B127A}"/>
+    <workbookView xWindow="1400" yWindow="460" windowWidth="25680" windowHeight="15920" xr2:uid="{4B2E00A5-7125-EC4E-9EAD-C4CEE86B127A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4221" uniqueCount="3565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4284" uniqueCount="3614">
   <si>
     <t>Date</t>
   </si>
@@ -10728,6 +10728,153 @@
   </si>
   <si>
     <t>56:49</t>
+  </si>
+  <si>
+    <t>2020-12-04</t>
+  </si>
+  <si>
+    <t>51:20</t>
+  </si>
+  <si>
+    <t>2020-12-05</t>
+  </si>
+  <si>
+    <t>2020-12-06</t>
+  </si>
+  <si>
+    <t>2020-12-16</t>
+  </si>
+  <si>
+    <t>2020-12-21</t>
+  </si>
+  <si>
+    <t>2020-12-22</t>
+  </si>
+  <si>
+    <t>2020-12-23</t>
+  </si>
+  <si>
+    <t>2020-12-24</t>
+  </si>
+  <si>
+    <t>2020-12-26</t>
+  </si>
+  <si>
+    <t>2020-12-27</t>
+  </si>
+  <si>
+    <t>2020-12-28</t>
+  </si>
+  <si>
+    <t>46:35</t>
+  </si>
+  <si>
+    <t>2020-12-30</t>
+  </si>
+  <si>
+    <t>2020-12-31</t>
+  </si>
+  <si>
+    <t>2021-01-01</t>
+  </si>
+  <si>
+    <t>48:44</t>
+  </si>
+  <si>
+    <t>2021-01-02</t>
+  </si>
+  <si>
+    <t>53:35</t>
+  </si>
+  <si>
+    <t>2021-01-04</t>
+  </si>
+  <si>
+    <t>2021-01-05</t>
+  </si>
+  <si>
+    <t>54:13</t>
+  </si>
+  <si>
+    <t>2021-01-06</t>
+  </si>
+  <si>
+    <t>40:44</t>
+  </si>
+  <si>
+    <t>2021-01-07</t>
+  </si>
+  <si>
+    <t>1:06:54</t>
+  </si>
+  <si>
+    <t>2021-01-08</t>
+  </si>
+  <si>
+    <t>2021-01-09</t>
+  </si>
+  <si>
+    <t>1:17:22</t>
+  </si>
+  <si>
+    <t>2021-01-11</t>
+  </si>
+  <si>
+    <t>48:40</t>
+  </si>
+  <si>
+    <t>2021-01-12</t>
+  </si>
+  <si>
+    <t>50:45</t>
+  </si>
+  <si>
+    <t>2021-01-13</t>
+  </si>
+  <si>
+    <t>43:59</t>
+  </si>
+  <si>
+    <t>2021-01-15</t>
+  </si>
+  <si>
+    <t>1:02:49</t>
+  </si>
+  <si>
+    <t>2021-01-17</t>
+  </si>
+  <si>
+    <t>1:25:01</t>
+  </si>
+  <si>
+    <t>2021-01-18</t>
+  </si>
+  <si>
+    <t>2021-01-19</t>
+  </si>
+  <si>
+    <t>2021-01-20</t>
+  </si>
+  <si>
+    <t>56:09</t>
+  </si>
+  <si>
+    <t>2021-01-21</t>
+  </si>
+  <si>
+    <t>48:15</t>
+  </si>
+  <si>
+    <t>2021-01-22</t>
+  </si>
+  <si>
+    <t>50:19</t>
+  </si>
+  <si>
+    <t>2021-01-23</t>
+  </si>
+  <si>
+    <t>1:25:30</t>
   </si>
 </sst>
 </file>
@@ -11101,10 +11248,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BECE25-7878-7543-A5E4-1B4438F2AAC2}">
-  <dimension ref="A1:E2681"/>
+  <dimension ref="A1:E2713"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2651" workbookViewId="0">
-      <selection activeCell="C2682" sqref="C2682"/>
+    <sheetView tabSelected="1" topLeftCell="A2685" workbookViewId="0">
+      <selection activeCell="C2714" sqref="C2714"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38845,6 +38992,355 @@
         <v>3564</v>
       </c>
     </row>
+    <row r="2682" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2682" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="B2682" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="C2682" s="2" t="s">
+        <v>3566</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2683" s="2" t="s">
+        <v>3567</v>
+      </c>
+      <c r="B2683" s="1">
+        <v>6.01</v>
+      </c>
+      <c r="C2683" s="2" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2684" s="2" t="s">
+        <v>3568</v>
+      </c>
+      <c r="B2684" s="1">
+        <v>2.68</v>
+      </c>
+      <c r="C2684" s="2" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2685" s="2" t="s">
+        <v>3569</v>
+      </c>
+      <c r="B2685" s="1">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2686" s="2" t="s">
+        <v>3570</v>
+      </c>
+      <c r="B2686" s="1">
+        <v>5.69</v>
+      </c>
+      <c r="C2686" s="2" t="s">
+        <v>3306</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2687" s="2" t="s">
+        <v>3571</v>
+      </c>
+      <c r="B2687" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2687" s="2" t="s">
+        <v>2609</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2688" s="2" t="s">
+        <v>3572</v>
+      </c>
+      <c r="B2688" s="1">
+        <v>7.14</v>
+      </c>
+      <c r="C2688" s="2" t="s">
+        <v>2959</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2689" s="2" t="s">
+        <v>3573</v>
+      </c>
+      <c r="B2689" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="C2689" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2690" s="2" t="s">
+        <v>3574</v>
+      </c>
+      <c r="B2690" s="1">
+        <v>7.07</v>
+      </c>
+      <c r="C2690" s="2" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2691" s="2" t="s">
+        <v>3575</v>
+      </c>
+      <c r="B2691" s="1">
+        <v>8.41</v>
+      </c>
+      <c r="C2691" s="2" t="s">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2692" s="2" t="s">
+        <v>3576</v>
+      </c>
+      <c r="B2692" s="1">
+        <v>7</v>
+      </c>
+      <c r="C2692" s="2" t="s">
+        <v>3577</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2693" s="2" t="s">
+        <v>3578</v>
+      </c>
+      <c r="B2693" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="C2693" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2694" s="2" t="s">
+        <v>3579</v>
+      </c>
+      <c r="B2694" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2694" s="2" t="s">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2695" s="2" t="s">
+        <v>3580</v>
+      </c>
+      <c r="B2695" s="1">
+        <v>6.82</v>
+      </c>
+      <c r="C2695" s="2" t="s">
+        <v>3581</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2696" s="2" t="s">
+        <v>3582</v>
+      </c>
+      <c r="B2696" s="1">
+        <v>7.09</v>
+      </c>
+      <c r="C2696" s="2" t="s">
+        <v>3583</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2697" s="2" t="s">
+        <v>3584</v>
+      </c>
+      <c r="B2697" s="1">
+        <v>7</v>
+      </c>
+      <c r="C2697" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2698" s="2" t="s">
+        <v>3585</v>
+      </c>
+      <c r="B2698" s="1">
+        <v>7.43</v>
+      </c>
+      <c r="C2698" s="2" t="s">
+        <v>3586</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2699" s="2" t="s">
+        <v>3587</v>
+      </c>
+      <c r="B2699" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2699" s="2" t="s">
+        <v>3588</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2700" s="2" t="s">
+        <v>3589</v>
+      </c>
+      <c r="B2700" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2700" s="2" t="s">
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2701" s="2" t="s">
+        <v>3591</v>
+      </c>
+      <c r="B2701" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2701" s="2" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2702" s="2" t="s">
+        <v>3592</v>
+      </c>
+      <c r="B2702" s="1">
+        <v>11.12</v>
+      </c>
+      <c r="C2702" s="2" t="s">
+        <v>3593</v>
+      </c>
+    </row>
+    <row r="2703" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2703" s="2" t="s">
+        <v>3594</v>
+      </c>
+      <c r="B2703" s="1">
+        <v>7.49</v>
+      </c>
+      <c r="C2703" s="2" t="s">
+        <v>3595</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2704" s="2" t="s">
+        <v>3596</v>
+      </c>
+      <c r="B2704" s="1">
+        <v>7.64</v>
+      </c>
+      <c r="C2704" s="2" t="s">
+        <v>3597</v>
+      </c>
+    </row>
+    <row r="2705" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2705" s="2" t="s">
+        <v>3598</v>
+      </c>
+      <c r="B2705" s="1">
+        <v>6.01</v>
+      </c>
+      <c r="C2705" s="2" t="s">
+        <v>3599</v>
+      </c>
+    </row>
+    <row r="2706" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2706" s="2" t="s">
+        <v>3600</v>
+      </c>
+      <c r="B2706" s="1">
+        <v>8.42</v>
+      </c>
+      <c r="C2706" s="2" t="s">
+        <v>3601</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2707" s="2" t="s">
+        <v>3602</v>
+      </c>
+      <c r="B2707" s="1">
+        <v>11.11</v>
+      </c>
+      <c r="C2707" s="2" t="s">
+        <v>3603</v>
+      </c>
+    </row>
+    <row r="2708" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2708" s="2" t="s">
+        <v>3604</v>
+      </c>
+      <c r="B2708" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="C2708" s="2" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2709" s="2" t="s">
+        <v>3605</v>
+      </c>
+      <c r="B2709" s="1">
+        <v>7.42</v>
+      </c>
+      <c r="C2709" s="2" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2710" s="2" t="s">
+        <v>3606</v>
+      </c>
+      <c r="B2710" s="1">
+        <v>8.26</v>
+      </c>
+      <c r="C2710" s="2" t="s">
+        <v>3607</v>
+      </c>
+    </row>
+    <row r="2711" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2711" s="2" t="s">
+        <v>3608</v>
+      </c>
+      <c r="B2711" s="1">
+        <v>7</v>
+      </c>
+      <c r="C2711" s="2" t="s">
+        <v>3609</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2712" s="2" t="s">
+        <v>3610</v>
+      </c>
+      <c r="B2712" s="1">
+        <v>7.18</v>
+      </c>
+      <c r="C2712" s="2" t="s">
+        <v>3611</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2713" s="2" t="s">
+        <v>3612</v>
+      </c>
+      <c r="B2713" s="1">
+        <v>13.1</v>
+      </c>
+      <c r="C2713" s="2" t="s">
+        <v>3613</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
I ran a half marathon
</commit_message>
<xml_diff>
--- a/Running_Log.xlsx
+++ b/Running_Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlexDolwick/dolwick_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D773CA-71B7-7640-823B-372066532687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D494D2E-FBBF-0D47-8353-2B6A6DC13AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="460" windowWidth="25680" windowHeight="15920" xr2:uid="{4B2E00A5-7125-EC4E-9EAD-C4CEE86B127A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4572" uniqueCount="3844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4612" uniqueCount="3875">
   <si>
     <t>Date</t>
   </si>
@@ -11565,6 +11565,99 @@
   </si>
   <si>
     <t>1:12:50</t>
+  </si>
+  <si>
+    <t>2021-09-07</t>
+  </si>
+  <si>
+    <t>2021-09-08</t>
+  </si>
+  <si>
+    <t>1:08:54</t>
+  </si>
+  <si>
+    <t>2021-09-09</t>
+  </si>
+  <si>
+    <t>47:10</t>
+  </si>
+  <si>
+    <t>2021-09-10</t>
+  </si>
+  <si>
+    <t>2021-09-11</t>
+  </si>
+  <si>
+    <t>16:28</t>
+  </si>
+  <si>
+    <t>2021-09-13</t>
+  </si>
+  <si>
+    <t>1:08:43</t>
+  </si>
+  <si>
+    <t>2021-09-14</t>
+  </si>
+  <si>
+    <t>47:33</t>
+  </si>
+  <si>
+    <t>2021-09-15</t>
+  </si>
+  <si>
+    <t>1:06:32</t>
+  </si>
+  <si>
+    <t>2021-09-16</t>
+  </si>
+  <si>
+    <t>2021-09-17</t>
+  </si>
+  <si>
+    <t>2021-09-18</t>
+  </si>
+  <si>
+    <t>1:01:50</t>
+  </si>
+  <si>
+    <t>2021-09-19</t>
+  </si>
+  <si>
+    <t>1:26:20</t>
+  </si>
+  <si>
+    <t>2021-09-21</t>
+  </si>
+  <si>
+    <t>2021-09-24</t>
+  </si>
+  <si>
+    <t>44:25</t>
+  </si>
+  <si>
+    <t>2021-09-26</t>
+  </si>
+  <si>
+    <t>2021-09-27</t>
+  </si>
+  <si>
+    <t>27:09</t>
+  </si>
+  <si>
+    <t>2021-09-29</t>
+  </si>
+  <si>
+    <t>41:22</t>
+  </si>
+  <si>
+    <t>2021-10-01</t>
+  </si>
+  <si>
+    <t>2021-10-02</t>
+  </si>
+  <si>
+    <t>1:16:48</t>
   </si>
 </sst>
 </file>
@@ -11938,10 +12031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BECE25-7878-7543-A5E4-1B4438F2AAC2}">
-  <dimension ref="A1:E2858"/>
+  <dimension ref="A1:E2879"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2841" workbookViewId="0">
-      <selection activeCell="B2861" sqref="B2861"/>
+    <sheetView tabSelected="1" topLeftCell="A2850" workbookViewId="0">
+      <selection activeCell="F2855" sqref="F2855"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41620,6 +41713,231 @@
         <v>3843</v>
       </c>
     </row>
+    <row r="2859" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2859" s="2" t="s">
+        <v>3844</v>
+      </c>
+      <c r="B2859" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2859" s="2" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="2860" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2860" s="2" t="s">
+        <v>3845</v>
+      </c>
+      <c r="B2860" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2860" s="2" t="s">
+        <v>3846</v>
+      </c>
+    </row>
+    <row r="2861" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2861" s="2" t="s">
+        <v>3847</v>
+      </c>
+      <c r="B2861" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2861" s="2" t="s">
+        <v>3848</v>
+      </c>
+    </row>
+    <row r="2862" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2862" s="2" t="s">
+        <v>3849</v>
+      </c>
+      <c r="B2862" s="1">
+        <v>7.83</v>
+      </c>
+      <c r="C2862" s="2" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="2863" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2863" s="2" t="s">
+        <v>3850</v>
+      </c>
+      <c r="B2863" s="1">
+        <v>3.11</v>
+      </c>
+      <c r="C2863" s="2" t="s">
+        <v>3851</v>
+      </c>
+    </row>
+    <row r="2864" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2864" s="2" t="s">
+        <v>3850</v>
+      </c>
+      <c r="B2864" s="1">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="2865" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2865" s="2" t="s">
+        <v>3852</v>
+      </c>
+      <c r="B2865" s="1">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="C2865" s="2" t="s">
+        <v>3853</v>
+      </c>
+    </row>
+    <row r="2866" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2866" s="2" t="s">
+        <v>3854</v>
+      </c>
+      <c r="B2866" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2866" s="2" t="s">
+        <v>3855</v>
+      </c>
+    </row>
+    <row r="2867" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2867" s="2" t="s">
+        <v>3856</v>
+      </c>
+      <c r="B2867" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2867" s="2" t="s">
+        <v>3857</v>
+      </c>
+    </row>
+    <row r="2868" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2868" s="2" t="s">
+        <v>3858</v>
+      </c>
+      <c r="B2868" s="1">
+        <v>6.02</v>
+      </c>
+      <c r="C2868" s="2" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="2869" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2869" s="2" t="s">
+        <v>3859</v>
+      </c>
+      <c r="B2869" s="1">
+        <v>4.01</v>
+      </c>
+      <c r="C2869" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="2870" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2870" s="2" t="s">
+        <v>3860</v>
+      </c>
+      <c r="B2870" s="1">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="C2870" s="2" t="s">
+        <v>3861</v>
+      </c>
+    </row>
+    <row r="2871" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2871" s="2" t="s">
+        <v>3862</v>
+      </c>
+      <c r="B2871" s="1">
+        <v>13.1</v>
+      </c>
+      <c r="C2871" s="2" t="s">
+        <v>3863</v>
+      </c>
+    </row>
+    <row r="2872" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2872" s="2" t="s">
+        <v>3864</v>
+      </c>
+      <c r="B2872" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="C2872" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="2873" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2873" s="2" t="s">
+        <v>3865</v>
+      </c>
+      <c r="B2873" s="1">
+        <v>6.34</v>
+      </c>
+      <c r="C2873" s="2" t="s">
+        <v>3866</v>
+      </c>
+    </row>
+    <row r="2874" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2874" s="2" t="s">
+        <v>3867</v>
+      </c>
+      <c r="B2874" s="1">
+        <v>7.03</v>
+      </c>
+      <c r="C2874" s="2" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="2875" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2875" s="2" t="s">
+        <v>3868</v>
+      </c>
+      <c r="B2875" s="1">
+        <v>4.04</v>
+      </c>
+      <c r="C2875" s="2" t="s">
+        <v>3869</v>
+      </c>
+    </row>
+    <row r="2876" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2876" s="2" t="s">
+        <v>3870</v>
+      </c>
+      <c r="B2876" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2876" s="2" t="s">
+        <v>3871</v>
+      </c>
+    </row>
+    <row r="2877" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2877" s="2" t="s">
+        <v>3872</v>
+      </c>
+      <c r="B2877" s="1">
+        <v>4.01</v>
+      </c>
+      <c r="C2877" s="2" t="s">
+        <v>2288</v>
+      </c>
+    </row>
+    <row r="2878" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2878" s="2" t="s">
+        <v>3873</v>
+      </c>
+      <c r="B2878" s="1">
+        <v>13.11</v>
+      </c>
+      <c r="C2878" s="2" t="s">
+        <v>3874</v>
+      </c>
+    </row>
+    <row r="2879" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2879" s="2" t="s">
+        <v>3873</v>
+      </c>
+      <c r="B2879" s="1">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
minor fixes / 25oct2021 update
</commit_message>
<xml_diff>
--- a/Running_Log.xlsx
+++ b/Running_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlexDolwick/dolwick_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D09C1E4-CE13-144A-9833-55E3E1BA547E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBD1BDB-318B-8542-AB7A-E76A6CC8AAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="460" windowWidth="25680" windowHeight="15920" xr2:uid="{4B2E00A5-7125-EC4E-9EAD-C4CEE86B127A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4620" uniqueCount="3882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4624" uniqueCount="3886">
   <si>
     <t>Date</t>
   </si>
@@ -10508,9 +10508,6 @@
     <t>2020-10-14</t>
   </si>
   <si>
-    <t>2020-10-13</t>
-  </si>
-  <si>
     <t>42:16</t>
   </si>
   <si>
@@ -11679,6 +11676,21 @@
   </si>
   <si>
     <t>30:55</t>
+  </si>
+  <si>
+    <t>2021-10-23</t>
+  </si>
+  <si>
+    <t>53:42</t>
+  </si>
+  <si>
+    <t>2021-10-25</t>
+  </si>
+  <si>
+    <t>40:54</t>
+  </si>
+  <si>
+    <t>2020-10-12</t>
   </si>
 </sst>
 </file>
@@ -12052,10 +12064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BECE25-7878-7543-A5E4-1B4438F2AAC2}">
-  <dimension ref="A1:E2883"/>
+  <dimension ref="A1:E2885"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2856" workbookViewId="0">
-      <selection activeCell="C2884" sqref="C2884"/>
+    <sheetView tabSelected="1" topLeftCell="A1897" workbookViewId="0">
+      <selection activeCell="D1918" sqref="D1918"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32179,7 +32191,7 @@
         <v>2518</v>
       </c>
       <c r="B1915" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1915" s="2" t="s">
         <v>1982</v>
@@ -39303,13 +39315,13 @@
     </row>
     <row r="2637" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2637" s="2" t="s">
-        <v>3491</v>
+        <v>3885</v>
       </c>
       <c r="B2637" s="1">
         <v>5.25</v>
       </c>
       <c r="C2637" s="2" t="s">
-        <v>3492</v>
+        <v>3491</v>
       </c>
     </row>
     <row r="2638" spans="1:3" x14ac:dyDescent="0.2">
@@ -39320,12 +39332,12 @@
         <v>10.17</v>
       </c>
       <c r="C2638" s="2" t="s">
-        <v>3493</v>
+        <v>3492</v>
       </c>
     </row>
     <row r="2639" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2639" s="2" t="s">
-        <v>3494</v>
+        <v>3493</v>
       </c>
       <c r="B2639" s="1">
         <v>5.13</v>
@@ -39336,7 +39348,7 @@
     </row>
     <row r="2640" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2640" s="2" t="s">
-        <v>3494</v>
+        <v>3493</v>
       </c>
       <c r="B2640" s="1">
         <v>5.01</v>
@@ -39347,29 +39359,29 @@
     </row>
     <row r="2641" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2641" s="2" t="s">
-        <v>3495</v>
+        <v>3494</v>
       </c>
       <c r="B2641" s="1">
         <v>10.06</v>
       </c>
       <c r="C2641" s="2" t="s">
-        <v>3496</v>
+        <v>3495</v>
       </c>
     </row>
     <row r="2642" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2642" s="2" t="s">
-        <v>3497</v>
+        <v>3496</v>
       </c>
       <c r="B2642" s="1">
         <v>15.37</v>
       </c>
       <c r="C2642" s="2" t="s">
-        <v>3498</v>
+        <v>3497</v>
       </c>
     </row>
     <row r="2643" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2643" s="2" t="s">
-        <v>3499</v>
+        <v>3498</v>
       </c>
       <c r="B2643" s="1">
         <v>8.81</v>
@@ -39380,18 +39392,18 @@
     </row>
     <row r="2644" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2644" s="2" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
       <c r="B2644" s="1">
         <v>8.0399999999999991</v>
       </c>
       <c r="C2644" s="2" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="2645" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2645" s="2" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="B2645" s="1">
         <v>8.34</v>
@@ -39402,18 +39414,18 @@
     </row>
     <row r="2646" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2646" s="2" t="s">
-        <v>3503</v>
+        <v>3502</v>
       </c>
       <c r="B2646" s="1">
         <v>6.55</v>
       </c>
       <c r="C2646" s="2" t="s">
-        <v>3504</v>
+        <v>3503</v>
       </c>
     </row>
     <row r="2647" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2647" s="2" t="s">
-        <v>3505</v>
+        <v>3504</v>
       </c>
       <c r="B2647" s="1">
         <v>8.07</v>
@@ -39424,7 +39436,7 @@
     </row>
     <row r="2648" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2648" s="2" t="s">
-        <v>3506</v>
+        <v>3505</v>
       </c>
       <c r="B2648" s="1">
         <v>7.24</v>
@@ -39435,18 +39447,18 @@
     </row>
     <row r="2649" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2649" s="2" t="s">
-        <v>3507</v>
+        <v>3506</v>
       </c>
       <c r="B2649" s="1">
         <v>10.34</v>
       </c>
       <c r="C2649" s="2" t="s">
-        <v>3508</v>
+        <v>3507</v>
       </c>
     </row>
     <row r="2650" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2650" s="2" t="s">
-        <v>3509</v>
+        <v>3508</v>
       </c>
       <c r="B2650" s="1">
         <v>9.69</v>
@@ -39457,18 +39469,18 @@
     </row>
     <row r="2651" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2651" s="2" t="s">
-        <v>3510</v>
+        <v>3509</v>
       </c>
       <c r="B2651" s="1">
         <v>9.66</v>
       </c>
       <c r="C2651" s="2" t="s">
-        <v>3511</v>
+        <v>3510</v>
       </c>
     </row>
     <row r="2652" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2652" s="2" t="s">
-        <v>3512</v>
+        <v>3511</v>
       </c>
       <c r="B2652" s="1">
         <v>6.62</v>
@@ -39479,40 +39491,40 @@
     </row>
     <row r="2653" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2653" s="2" t="s">
-        <v>3513</v>
+        <v>3512</v>
       </c>
       <c r="B2653" s="1">
         <v>15.13</v>
       </c>
       <c r="C2653" s="2" t="s">
-        <v>3514</v>
+        <v>3513</v>
       </c>
     </row>
     <row r="2654" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2654" s="2" t="s">
-        <v>3515</v>
+        <v>3514</v>
       </c>
       <c r="B2654" s="1">
         <v>10.029999999999999</v>
       </c>
       <c r="C2654" s="2" t="s">
-        <v>3516</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="2655" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2655" s="2" t="s">
-        <v>3517</v>
+        <v>3516</v>
       </c>
       <c r="B2655" s="1">
         <v>10.37</v>
       </c>
       <c r="C2655" s="2" t="s">
-        <v>3518</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="2656" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2656" s="2" t="s">
-        <v>3519</v>
+        <v>3518</v>
       </c>
       <c r="B2656" s="1">
         <v>7.6</v>
@@ -39523,73 +39535,73 @@
     </row>
     <row r="2657" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2657" s="2" t="s">
-        <v>3520</v>
+        <v>3519</v>
       </c>
       <c r="B2657" s="1">
         <v>8.02</v>
       </c>
       <c r="C2657" s="2" t="s">
-        <v>3521</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="2658" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2658" s="2" t="s">
-        <v>3522</v>
+        <v>3521</v>
       </c>
       <c r="B2658" s="1">
         <v>9.2799999999999994</v>
       </c>
       <c r="C2658" s="2" t="s">
-        <v>3523</v>
+        <v>3522</v>
       </c>
     </row>
     <row r="2659" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2659" s="2" t="s">
-        <v>3524</v>
+        <v>3523</v>
       </c>
       <c r="B2659" s="1">
         <v>9.7200000000000006</v>
       </c>
       <c r="C2659" s="2" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
     </row>
     <row r="2660" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2660" s="2" t="s">
-        <v>3526</v>
+        <v>3525</v>
       </c>
       <c r="B2660" s="1">
         <v>16.3</v>
       </c>
       <c r="C2660" s="2" t="s">
-        <v>3527</v>
+        <v>3526</v>
       </c>
     </row>
     <row r="2661" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2661" s="2" t="s">
-        <v>3528</v>
+        <v>3527</v>
       </c>
       <c r="B2661" s="1">
         <v>8.24</v>
       </c>
       <c r="C2661" s="2" t="s">
-        <v>3529</v>
+        <v>3528</v>
       </c>
     </row>
     <row r="2662" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2662" s="2" t="s">
-        <v>3530</v>
+        <v>3529</v>
       </c>
       <c r="B2662" s="1">
         <v>11.03</v>
       </c>
       <c r="C2662" s="2" t="s">
-        <v>3531</v>
+        <v>3530</v>
       </c>
     </row>
     <row r="2663" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2663" s="2" t="s">
-        <v>3532</v>
+        <v>3531</v>
       </c>
       <c r="B2663" s="1">
         <v>11.01</v>
@@ -39600,51 +39612,51 @@
     </row>
     <row r="2664" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2664" s="2" t="s">
-        <v>3533</v>
+        <v>3532</v>
       </c>
       <c r="B2664" s="1">
         <v>6.5</v>
       </c>
       <c r="C2664" s="2" t="s">
-        <v>3534</v>
+        <v>3533</v>
       </c>
     </row>
     <row r="2665" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2665" s="2" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="B2665" s="1">
         <v>13.51</v>
       </c>
       <c r="C2665" s="2" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
     </row>
     <row r="2666" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2666" s="2" t="s">
-        <v>3537</v>
+        <v>3536</v>
       </c>
       <c r="B2666" s="1">
         <v>6.01</v>
       </c>
       <c r="C2666" s="2" t="s">
-        <v>3538</v>
+        <v>3537</v>
       </c>
     </row>
     <row r="2667" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2667" s="2" t="s">
-        <v>3539</v>
+        <v>3538</v>
       </c>
       <c r="B2667" s="1">
         <v>10.51</v>
       </c>
       <c r="C2667" s="2" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
     </row>
     <row r="2668" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2668" s="2" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
       <c r="B2668" s="1">
         <v>10</v>
@@ -39655,7 +39667,7 @@
     </row>
     <row r="2669" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2669" s="2" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
       <c r="B2669" s="1">
         <v>6.65</v>
@@ -39666,7 +39678,7 @@
     </row>
     <row r="2670" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2670" s="2" t="s">
-        <v>3543</v>
+        <v>3542</v>
       </c>
       <c r="B2670" s="1">
         <v>10</v>
@@ -39677,62 +39689,62 @@
     </row>
     <row r="2671" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2671" s="2" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="B2671" s="1">
         <v>17</v>
       </c>
       <c r="C2671" s="2" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
     </row>
     <row r="2672" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2672" s="2" t="s">
-        <v>3546</v>
+        <v>3545</v>
       </c>
       <c r="B2672" s="1">
         <v>6</v>
       </c>
       <c r="C2672" s="2" t="s">
-        <v>3547</v>
+        <v>3546</v>
       </c>
     </row>
     <row r="2673" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2673" s="2" t="s">
-        <v>3548</v>
+        <v>3547</v>
       </c>
       <c r="B2673" s="1">
         <v>9.27</v>
       </c>
       <c r="C2673" s="2" t="s">
-        <v>3549</v>
+        <v>3548</v>
       </c>
     </row>
     <row r="2674" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2674" s="2" t="s">
-        <v>3550</v>
+        <v>3549</v>
       </c>
       <c r="B2674" s="1">
         <v>6</v>
       </c>
       <c r="C2674" s="2" t="s">
-        <v>3551</v>
+        <v>3550</v>
       </c>
     </row>
     <row r="2675" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2675" s="2" t="s">
-        <v>3552</v>
+        <v>3551</v>
       </c>
       <c r="B2675" s="1">
         <v>7.32</v>
       </c>
       <c r="C2675" s="2" t="s">
-        <v>3553</v>
+        <v>3552</v>
       </c>
     </row>
     <row r="2676" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2676" s="2" t="s">
-        <v>3554</v>
+        <v>3553</v>
       </c>
       <c r="B2676" s="1">
         <v>6</v>
@@ -39743,73 +39755,73 @@
     </row>
     <row r="2677" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2677" s="2" t="s">
-        <v>3555</v>
+        <v>3554</v>
       </c>
       <c r="B2677" s="1">
         <v>7.52</v>
       </c>
       <c r="C2677" s="2" t="s">
-        <v>3556</v>
+        <v>3555</v>
       </c>
     </row>
     <row r="2678" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2678" s="2" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
       <c r="B2678" s="1">
         <v>7.34</v>
       </c>
       <c r="C2678" s="2" t="s">
-        <v>3558</v>
+        <v>3557</v>
       </c>
     </row>
     <row r="2679" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2679" s="2" t="s">
-        <v>3559</v>
+        <v>3558</v>
       </c>
       <c r="B2679" s="1">
         <v>6.13</v>
       </c>
       <c r="C2679" s="2" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
     </row>
     <row r="2680" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2680" s="2" t="s">
-        <v>3561</v>
+        <v>3560</v>
       </c>
       <c r="B2680" s="1">
         <v>6.29</v>
       </c>
       <c r="C2680" s="2" t="s">
-        <v>3562</v>
+        <v>3561</v>
       </c>
     </row>
     <row r="2681" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2681" s="2" t="s">
-        <v>3563</v>
+        <v>3562</v>
       </c>
       <c r="B2681" s="1">
         <v>7.59</v>
       </c>
       <c r="C2681" s="2" t="s">
-        <v>3564</v>
+        <v>3563</v>
       </c>
     </row>
     <row r="2682" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2682" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="B2682" s="1">
         <v>7.4</v>
       </c>
       <c r="C2682" s="2" t="s">
-        <v>3566</v>
+        <v>3565</v>
       </c>
     </row>
     <row r="2683" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2683" s="2" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="B2683" s="1">
         <v>6.01</v>
@@ -39820,7 +39832,7 @@
     </row>
     <row r="2684" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2684" s="2" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
       <c r="B2684" s="1">
         <v>2.68</v>
@@ -39831,7 +39843,7 @@
     </row>
     <row r="2685" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2685" s="2" t="s">
-        <v>3569</v>
+        <v>3568</v>
       </c>
       <c r="B2685" s="1">
         <v>2.84</v>
@@ -39839,7 +39851,7 @@
     </row>
     <row r="2686" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2686" s="2" t="s">
-        <v>3570</v>
+        <v>3569</v>
       </c>
       <c r="B2686" s="1">
         <v>5.69</v>
@@ -39850,7 +39862,7 @@
     </row>
     <row r="2687" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2687" s="2" t="s">
-        <v>3571</v>
+        <v>3570</v>
       </c>
       <c r="B2687" s="1">
         <v>5</v>
@@ -39861,7 +39873,7 @@
     </row>
     <row r="2688" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2688" s="2" t="s">
-        <v>3572</v>
+        <v>3571</v>
       </c>
       <c r="B2688" s="1">
         <v>7.14</v>
@@ -39872,7 +39884,7 @@
     </row>
     <row r="2689" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2689" s="2" t="s">
-        <v>3573</v>
+        <v>3572</v>
       </c>
       <c r="B2689" s="1">
         <v>4.6500000000000004</v>
@@ -39883,7 +39895,7 @@
     </row>
     <row r="2690" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2690" s="2" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
       <c r="B2690" s="1">
         <v>7.07</v>
@@ -39894,7 +39906,7 @@
     </row>
     <row r="2691" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2691" s="2" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="B2691" s="1">
         <v>8.41</v>
@@ -39905,18 +39917,18 @@
     </row>
     <row r="2692" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2692" s="2" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
       <c r="B2692" s="1">
         <v>7</v>
       </c>
       <c r="C2692" s="2" t="s">
-        <v>3577</v>
+        <v>3576</v>
       </c>
     </row>
     <row r="2693" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2693" s="2" t="s">
-        <v>3578</v>
+        <v>3577</v>
       </c>
       <c r="B2693" s="1">
         <v>7.5</v>
@@ -39927,7 +39939,7 @@
     </row>
     <row r="2694" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2694" s="2" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="B2694" s="1">
         <v>6</v>
@@ -39938,29 +39950,29 @@
     </row>
     <row r="2695" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2695" s="2" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="B2695" s="1">
         <v>6.82</v>
       </c>
       <c r="C2695" s="2" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
     </row>
     <row r="2696" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2696" s="2" t="s">
-        <v>3582</v>
+        <v>3581</v>
       </c>
       <c r="B2696" s="1">
         <v>7.09</v>
       </c>
       <c r="C2696" s="2" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
     </row>
     <row r="2697" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2697" s="2" t="s">
-        <v>3584</v>
+        <v>3583</v>
       </c>
       <c r="B2697" s="1">
         <v>7</v>
@@ -39971,40 +39983,40 @@
     </row>
     <row r="2698" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2698" s="2" t="s">
-        <v>3585</v>
+        <v>3584</v>
       </c>
       <c r="B2698" s="1">
         <v>7.43</v>
       </c>
       <c r="C2698" s="2" t="s">
-        <v>3586</v>
+        <v>3585</v>
       </c>
     </row>
     <row r="2699" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2699" s="2" t="s">
-        <v>3587</v>
+        <v>3586</v>
       </c>
       <c r="B2699" s="1">
         <v>6</v>
       </c>
       <c r="C2699" s="2" t="s">
-        <v>3588</v>
+        <v>3587</v>
       </c>
     </row>
     <row r="2700" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2700" s="2" t="s">
-        <v>3589</v>
+        <v>3588</v>
       </c>
       <c r="B2700" s="1">
         <v>8</v>
       </c>
       <c r="C2700" s="2" t="s">
-        <v>3590</v>
+        <v>3589</v>
       </c>
     </row>
     <row r="2701" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2701" s="2" t="s">
-        <v>3591</v>
+        <v>3590</v>
       </c>
       <c r="B2701" s="1">
         <v>6</v>
@@ -40015,73 +40027,73 @@
     </row>
     <row r="2702" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2702" s="2" t="s">
-        <v>3592</v>
+        <v>3591</v>
       </c>
       <c r="B2702" s="1">
         <v>11.12</v>
       </c>
       <c r="C2702" s="2" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="2703" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2703" s="2" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
       <c r="B2703" s="1">
         <v>7.49</v>
       </c>
       <c r="C2703" s="2" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
     </row>
     <row r="2704" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2704" s="2" t="s">
-        <v>3596</v>
+        <v>3595</v>
       </c>
       <c r="B2704" s="1">
         <v>7.64</v>
       </c>
       <c r="C2704" s="2" t="s">
-        <v>3597</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="2705" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2705" s="2" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="B2705" s="1">
         <v>6.01</v>
       </c>
       <c r="C2705" s="2" t="s">
-        <v>3599</v>
+        <v>3598</v>
       </c>
     </row>
     <row r="2706" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2706" s="2" t="s">
-        <v>3600</v>
+        <v>3599</v>
       </c>
       <c r="B2706" s="1">
         <v>8.42</v>
       </c>
       <c r="C2706" s="2" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="2707" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2707" s="2" t="s">
-        <v>3602</v>
+        <v>3601</v>
       </c>
       <c r="B2707" s="1">
         <v>11.11</v>
       </c>
       <c r="C2707" s="2" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="2708" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2708" s="2" t="s">
-        <v>3604</v>
+        <v>3603</v>
       </c>
       <c r="B2708" s="1">
         <v>7.75</v>
@@ -40092,7 +40104,7 @@
     </row>
     <row r="2709" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2709" s="2" t="s">
-        <v>3605</v>
+        <v>3604</v>
       </c>
       <c r="B2709" s="1">
         <v>7.42</v>
@@ -40103,62 +40115,62 @@
     </row>
     <row r="2710" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2710" s="2" t="s">
-        <v>3606</v>
+        <v>3605</v>
       </c>
       <c r="B2710" s="1">
         <v>8.26</v>
       </c>
       <c r="C2710" s="2" t="s">
-        <v>3607</v>
+        <v>3606</v>
       </c>
     </row>
     <row r="2711" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2711" s="2" t="s">
-        <v>3608</v>
+        <v>3607</v>
       </c>
       <c r="B2711" s="1">
         <v>7</v>
       </c>
       <c r="C2711" s="2" t="s">
-        <v>3609</v>
+        <v>3608</v>
       </c>
     </row>
     <row r="2712" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2712" s="2" t="s">
-        <v>3610</v>
+        <v>3609</v>
       </c>
       <c r="B2712" s="1">
         <v>7.18</v>
       </c>
       <c r="C2712" s="2" t="s">
-        <v>3611</v>
+        <v>3610</v>
       </c>
     </row>
     <row r="2713" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2713" s="2" t="s">
-        <v>3612</v>
+        <v>3611</v>
       </c>
       <c r="B2713" s="1">
         <v>13.1</v>
       </c>
       <c r="C2713" s="2" t="s">
-        <v>3613</v>
+        <v>3612</v>
       </c>
     </row>
     <row r="2714" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2714" s="2" t="s">
-        <v>3614</v>
+        <v>3613</v>
       </c>
       <c r="B2714" s="1">
         <v>6</v>
       </c>
       <c r="C2714" s="2" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="2715" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2715" s="2" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
       <c r="B2715" s="1">
         <v>9.41</v>
@@ -40169,29 +40181,29 @@
     </row>
     <row r="2716" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2716" s="2" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
       <c r="B2716" s="1">
         <v>7.43</v>
       </c>
       <c r="C2716" s="2" t="s">
-        <v>3618</v>
+        <v>3617</v>
       </c>
     </row>
     <row r="2717" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2717" s="2" t="s">
-        <v>3619</v>
+        <v>3618</v>
       </c>
       <c r="B2717" s="1">
         <v>8.44</v>
       </c>
       <c r="C2717" s="2" t="s">
-        <v>3620</v>
+        <v>3619</v>
       </c>
     </row>
     <row r="2718" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2718" s="2" t="s">
-        <v>3621</v>
+        <v>3620</v>
       </c>
       <c r="B2718" s="1">
         <v>7</v>
@@ -40202,40 +40214,40 @@
     </row>
     <row r="2719" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2719" s="2" t="s">
-        <v>3622</v>
+        <v>3621</v>
       </c>
       <c r="B2719" s="1">
         <v>7</v>
       </c>
       <c r="C2719" s="2" t="s">
-        <v>3623</v>
+        <v>3622</v>
       </c>
     </row>
     <row r="2720" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2720" s="2" t="s">
-        <v>3624</v>
+        <v>3623</v>
       </c>
       <c r="B2720" s="1">
         <v>15.04</v>
       </c>
       <c r="C2720" s="2" t="s">
-        <v>3625</v>
+        <v>3624</v>
       </c>
     </row>
     <row r="2721" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2721" s="2" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
       <c r="B2721" s="1">
         <v>5.57</v>
       </c>
       <c r="C2721" s="2" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="2722" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2722" s="2" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
       <c r="B2722" s="1">
         <v>6.44</v>
@@ -40246,51 +40258,51 @@
     </row>
     <row r="2723" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2723" s="2" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
       <c r="B2723" s="1">
         <v>7.1</v>
       </c>
       <c r="C2723" s="2" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
     </row>
     <row r="2724" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2724" s="2" t="s">
-        <v>3631</v>
+        <v>3630</v>
       </c>
       <c r="B2724" s="1">
         <v>8.31</v>
       </c>
       <c r="C2724" s="2" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
     </row>
     <row r="2725" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2725" s="2" t="s">
-        <v>3633</v>
+        <v>3632</v>
       </c>
       <c r="B2725" s="1">
         <v>8.3800000000000008</v>
       </c>
       <c r="C2725" s="2" t="s">
-        <v>3632</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="2726" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2726" s="2" t="s">
-        <v>3634</v>
+        <v>3633</v>
       </c>
       <c r="B2726" s="1">
         <v>8</v>
       </c>
       <c r="C2726" s="2" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="2727" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2727" s="2" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
       <c r="B2727" s="1">
         <v>7.01</v>
@@ -40301,7 +40313,7 @@
     </row>
     <row r="2728" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2728" s="2" t="s">
-        <v>3637</v>
+        <v>3636</v>
       </c>
       <c r="B2728" s="1">
         <v>7.2</v>
@@ -40312,7 +40324,7 @@
     </row>
     <row r="2729" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2729" s="2" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
       <c r="B2729" s="1">
         <v>5.13</v>
@@ -40323,51 +40335,51 @@
     </row>
     <row r="2730" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2730" s="2" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
       <c r="B2730" s="1">
         <v>5.62</v>
       </c>
       <c r="C2730" s="2" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="2731" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2731" s="2" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
       <c r="B2731" s="1">
         <v>5.23</v>
       </c>
       <c r="C2731" s="2" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
     </row>
     <row r="2732" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2732" s="2" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
       <c r="B2732" s="1">
         <v>6.34</v>
       </c>
       <c r="C2732" s="2" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
     </row>
     <row r="2733" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2733" s="2" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
       <c r="B2733" s="1">
         <v>5.27</v>
       </c>
       <c r="C2733" s="2" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="2734" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2734" s="2" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
       <c r="B2734" s="1">
         <v>2.23</v>
@@ -40378,18 +40390,18 @@
     </row>
     <row r="2735" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2735" s="2" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
       <c r="B2735" s="1">
         <v>6.24</v>
       </c>
       <c r="C2735" s="2" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
     </row>
     <row r="2736" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2736" s="2" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
       <c r="B2736" s="1">
         <v>6.26</v>
@@ -40400,7 +40412,7 @@
     </row>
     <row r="2737" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2737" s="2" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
       <c r="B2737" s="1">
         <v>5.78</v>
@@ -40411,18 +40423,18 @@
     </row>
     <row r="2738" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2738" s="2" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
       <c r="B2738" s="1">
         <v>10</v>
       </c>
       <c r="C2738" s="2" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="2739" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2739" s="2" t="s">
-        <v>3654</v>
+        <v>3653</v>
       </c>
       <c r="B2739" s="1">
         <v>8.3699999999999992</v>
@@ -40433,18 +40445,18 @@
     </row>
     <row r="2740" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2740" s="2" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="B2740" s="1">
         <v>6.3</v>
       </c>
       <c r="C2740" s="2" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
     </row>
     <row r="2741" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2741" s="2" t="s">
-        <v>3657</v>
+        <v>3656</v>
       </c>
       <c r="B2741" s="1">
         <v>9.0299999999999994</v>
@@ -40455,7 +40467,7 @@
     </row>
     <row r="2742" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2742" s="2" t="s">
-        <v>3658</v>
+        <v>3657</v>
       </c>
       <c r="B2742" s="1">
         <v>4.05</v>
@@ -40466,51 +40478,51 @@
     </row>
     <row r="2743" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2743" s="2" t="s">
-        <v>3659</v>
+        <v>3658</v>
       </c>
       <c r="B2743" s="1">
         <v>6.29</v>
       </c>
       <c r="C2743" s="2" t="s">
-        <v>3660</v>
+        <v>3659</v>
       </c>
     </row>
     <row r="2744" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2744" s="2" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="B2744" s="1">
         <v>12.54</v>
       </c>
       <c r="C2744" s="2" t="s">
-        <v>3662</v>
+        <v>3661</v>
       </c>
     </row>
     <row r="2745" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2745" s="2" t="s">
-        <v>3663</v>
+        <v>3662</v>
       </c>
       <c r="B2745" s="1">
         <v>6.25</v>
       </c>
       <c r="C2745" s="2" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
     </row>
     <row r="2746" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2746" s="2" t="s">
-        <v>3664</v>
+        <v>3663</v>
       </c>
       <c r="B2746" s="1">
         <v>3.08</v>
       </c>
       <c r="C2746" s="2" t="s">
-        <v>3665</v>
+        <v>3664</v>
       </c>
     </row>
     <row r="2747" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2747" s="2" t="s">
-        <v>3666</v>
+        <v>3665</v>
       </c>
       <c r="B2747" s="1">
         <v>4.0999999999999996</v>
@@ -40521,7 +40533,7 @@
     </row>
     <row r="2748" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2748" s="2" t="s">
-        <v>3667</v>
+        <v>3666</v>
       </c>
       <c r="B2748" s="1">
         <v>4.41</v>
@@ -40532,7 +40544,7 @@
     </row>
     <row r="2749" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2749" s="2" t="s">
-        <v>3668</v>
+        <v>3667</v>
       </c>
       <c r="B2749" s="1">
         <v>5</v>
@@ -40543,29 +40555,29 @@
     </row>
     <row r="2750" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2750" s="2" t="s">
-        <v>3669</v>
+        <v>3668</v>
       </c>
       <c r="B2750" s="1">
         <v>5.13</v>
       </c>
       <c r="C2750" s="2" t="s">
-        <v>3670</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="2751" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2751" s="2" t="s">
-        <v>3671</v>
+        <v>3670</v>
       </c>
       <c r="B2751" s="1">
         <v>5.12</v>
       </c>
       <c r="C2751" s="2" t="s">
-        <v>3672</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="2752" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2752" s="2" t="s">
-        <v>3673</v>
+        <v>3672</v>
       </c>
       <c r="B2752" s="1">
         <v>5.2</v>
@@ -40576,18 +40588,18 @@
     </row>
     <row r="2753" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2753" s="2" t="s">
-        <v>3674</v>
+        <v>3673</v>
       </c>
       <c r="B2753" s="1">
         <v>5.08</v>
       </c>
       <c r="C2753" s="2" t="s">
-        <v>3675</v>
+        <v>3674</v>
       </c>
     </row>
     <row r="2754" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2754" s="2" t="s">
-        <v>3676</v>
+        <v>3675</v>
       </c>
       <c r="B2754" s="1">
         <v>5</v>
@@ -40598,29 +40610,29 @@
     </row>
     <row r="2755" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2755" s="2" t="s">
-        <v>3677</v>
+        <v>3676</v>
       </c>
       <c r="B2755" s="1">
         <v>5.03</v>
       </c>
       <c r="C2755" s="2" t="s">
-        <v>3678</v>
+        <v>3677</v>
       </c>
     </row>
     <row r="2756" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2756" s="2" t="s">
-        <v>3679</v>
+        <v>3678</v>
       </c>
       <c r="B2756" s="1">
         <v>5.0199999999999996</v>
       </c>
       <c r="C2756" s="2" t="s">
-        <v>3680</v>
+        <v>3679</v>
       </c>
     </row>
     <row r="2757" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2757" s="2" t="s">
-        <v>3681</v>
+        <v>3680</v>
       </c>
       <c r="B2757" s="1">
         <v>5</v>
@@ -40631,18 +40643,18 @@
     </row>
     <row r="2758" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2758" s="2" t="s">
-        <v>3682</v>
+        <v>3681</v>
       </c>
       <c r="B2758" s="1">
         <v>5.5</v>
       </c>
       <c r="C2758" s="2" t="s">
-        <v>3683</v>
+        <v>3682</v>
       </c>
     </row>
     <row r="2759" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2759" s="2" t="s">
-        <v>3684</v>
+        <v>3683</v>
       </c>
       <c r="B2759" s="1">
         <v>5</v>
@@ -40653,18 +40665,18 @@
     </row>
     <row r="2760" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2760" s="2" t="s">
-        <v>3685</v>
+        <v>3684</v>
       </c>
       <c r="B2760" s="1">
         <v>5.43</v>
       </c>
       <c r="C2760" s="2" t="s">
-        <v>3686</v>
+        <v>3685</v>
       </c>
     </row>
     <row r="2761" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2761" s="2" t="s">
-        <v>3687</v>
+        <v>3686</v>
       </c>
       <c r="B2761" s="1">
         <v>4.3899999999999997</v>
@@ -40675,18 +40687,18 @@
     </row>
     <row r="2762" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2762" s="2" t="s">
-        <v>3688</v>
+        <v>3687</v>
       </c>
       <c r="B2762" s="1">
         <v>3.5</v>
       </c>
       <c r="C2762" s="2" t="s">
-        <v>3689</v>
+        <v>3688</v>
       </c>
     </row>
     <row r="2763" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2763" s="2" t="s">
-        <v>3690</v>
+        <v>3689</v>
       </c>
       <c r="B2763" s="1">
         <v>5</v>
@@ -40697,18 +40709,18 @@
     </row>
     <row r="2764" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2764" s="2" t="s">
-        <v>3691</v>
+        <v>3690</v>
       </c>
       <c r="B2764" s="1">
         <v>5.23</v>
       </c>
       <c r="C2764" s="2" t="s">
-        <v>3692</v>
+        <v>3691</v>
       </c>
     </row>
     <row r="2765" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2765" s="2" t="s">
-        <v>3693</v>
+        <v>3692</v>
       </c>
       <c r="B2765" s="1">
         <v>5.07</v>
@@ -40719,29 +40731,29 @@
     </row>
     <row r="2766" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2766" s="2" t="s">
-        <v>3694</v>
+        <v>3693</v>
       </c>
       <c r="B2766" s="1">
         <v>6.42</v>
       </c>
       <c r="C2766" s="2" t="s">
-        <v>3695</v>
+        <v>3694</v>
       </c>
     </row>
     <row r="2767" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2767" s="2" t="s">
-        <v>3696</v>
+        <v>3695</v>
       </c>
       <c r="B2767" s="1">
         <v>5.07</v>
       </c>
       <c r="C2767" s="2" t="s">
-        <v>3697</v>
+        <v>3696</v>
       </c>
     </row>
     <row r="2768" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2768" s="2" t="s">
-        <v>3698</v>
+        <v>3697</v>
       </c>
       <c r="B2768" s="1">
         <v>5</v>
@@ -40752,29 +40764,29 @@
     </row>
     <row r="2769" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2769" s="2" t="s">
-        <v>3699</v>
+        <v>3698</v>
       </c>
       <c r="B2769" s="1">
         <v>6.13</v>
       </c>
       <c r="C2769" s="2" t="s">
-        <v>3700</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="2770" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2770" s="2" t="s">
-        <v>3701</v>
+        <v>3700</v>
       </c>
       <c r="B2770" s="1">
         <v>7.14</v>
       </c>
       <c r="C2770" s="2" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
     </row>
     <row r="2771" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2771" s="2" t="s">
-        <v>3702</v>
+        <v>3701</v>
       </c>
       <c r="B2771" s="1">
         <v>6.61</v>
@@ -40785,7 +40797,7 @@
     </row>
     <row r="2772" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2772" s="2" t="s">
-        <v>3703</v>
+        <v>3702</v>
       </c>
       <c r="B2772" s="1">
         <v>7.05</v>
@@ -40793,18 +40805,18 @@
     </row>
     <row r="2773" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2773" s="2" t="s">
-        <v>3704</v>
+        <v>3703</v>
       </c>
       <c r="B2773" s="1">
         <v>4.13</v>
       </c>
       <c r="C2773" s="2" t="s">
-        <v>3705</v>
+        <v>3704</v>
       </c>
     </row>
     <row r="2774" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2774" s="2" t="s">
-        <v>3706</v>
+        <v>3705</v>
       </c>
       <c r="B2774" s="1">
         <v>7.5</v>
@@ -40815,128 +40827,128 @@
     </row>
     <row r="2775" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2775" s="2" t="s">
-        <v>3707</v>
+        <v>3706</v>
       </c>
       <c r="B2775" s="1">
         <v>7.03</v>
       </c>
       <c r="C2775" s="2" t="s">
-        <v>3708</v>
+        <v>3707</v>
       </c>
     </row>
     <row r="2776" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2776" s="2" t="s">
-        <v>3709</v>
+        <v>3708</v>
       </c>
       <c r="B2776" s="1">
         <v>6</v>
       </c>
       <c r="C2776" s="2" t="s">
-        <v>3710</v>
+        <v>3709</v>
       </c>
     </row>
     <row r="2777" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2777" s="2" t="s">
-        <v>3711</v>
+        <v>3710</v>
       </c>
       <c r="B2777" s="1">
         <v>7.28</v>
       </c>
       <c r="C2777" s="2" t="s">
-        <v>3712</v>
+        <v>3711</v>
       </c>
     </row>
     <row r="2778" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2778" s="2" t="s">
-        <v>3713</v>
+        <v>3712</v>
       </c>
       <c r="B2778" s="1">
         <v>7.13</v>
       </c>
       <c r="C2778" s="2" t="s">
-        <v>3714</v>
+        <v>3713</v>
       </c>
     </row>
     <row r="2779" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2779" s="2" t="s">
-        <v>3715</v>
+        <v>3714</v>
       </c>
       <c r="B2779" s="1">
         <v>5.19</v>
       </c>
       <c r="C2779" s="2" t="s">
-        <v>3716</v>
+        <v>3715</v>
       </c>
     </row>
     <row r="2780" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2780" s="2" t="s">
-        <v>3717</v>
+        <v>3716</v>
       </c>
       <c r="B2780" s="1">
         <v>8.7799999999999994</v>
       </c>
       <c r="C2780" s="2" t="s">
-        <v>3718</v>
+        <v>3717</v>
       </c>
     </row>
     <row r="2781" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2781" s="2" t="s">
-        <v>3719</v>
+        <v>3718</v>
       </c>
       <c r="B2781" s="1">
         <v>7.19</v>
       </c>
       <c r="C2781" s="2" t="s">
-        <v>3720</v>
+        <v>3719</v>
       </c>
     </row>
     <row r="2782" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2782" s="2" t="s">
-        <v>3721</v>
+        <v>3720</v>
       </c>
       <c r="B2782" s="1">
         <v>8.2100000000000009</v>
       </c>
       <c r="C2782" s="2" t="s">
-        <v>3722</v>
+        <v>3721</v>
       </c>
     </row>
     <row r="2783" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2783" s="2" t="s">
-        <v>3723</v>
+        <v>3722</v>
       </c>
       <c r="B2783" s="1">
         <v>5</v>
       </c>
       <c r="C2783" s="2" t="s">
-        <v>3675</v>
+        <v>3674</v>
       </c>
     </row>
     <row r="2784" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2784" s="2" t="s">
-        <v>3724</v>
+        <v>3723</v>
       </c>
       <c r="B2784" s="1">
         <v>5.21</v>
       </c>
       <c r="C2784" s="2" t="s">
-        <v>3725</v>
+        <v>3724</v>
       </c>
     </row>
     <row r="2785" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2785" s="2" t="s">
-        <v>3726</v>
+        <v>3725</v>
       </c>
       <c r="B2785" s="1">
         <v>5.55</v>
       </c>
       <c r="C2785" s="2" t="s">
-        <v>3727</v>
+        <v>3726</v>
       </c>
     </row>
     <row r="2786" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2786" s="2" t="s">
-        <v>3728</v>
+        <v>3727</v>
       </c>
       <c r="B2786" s="1">
         <v>6</v>
@@ -40947,7 +40959,7 @@
     </row>
     <row r="2787" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2787" s="2" t="s">
-        <v>3729</v>
+        <v>3728</v>
       </c>
       <c r="B2787" s="1">
         <v>7.05</v>
@@ -40958,7 +40970,7 @@
     </row>
     <row r="2788" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2788" s="2" t="s">
-        <v>3730</v>
+        <v>3729</v>
       </c>
       <c r="B2788" s="1">
         <v>8</v>
@@ -40969,40 +40981,40 @@
     </row>
     <row r="2789" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2789" s="2" t="s">
-        <v>3731</v>
+        <v>3730</v>
       </c>
       <c r="B2789" s="1">
         <v>6</v>
       </c>
       <c r="C2789" s="2" t="s">
-        <v>3732</v>
+        <v>3731</v>
       </c>
     </row>
     <row r="2790" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2790" s="2" t="s">
-        <v>3733</v>
+        <v>3732</v>
       </c>
       <c r="B2790" s="1">
         <v>7</v>
       </c>
       <c r="C2790" s="2" t="s">
-        <v>3734</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="2791" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2791" s="2" t="s">
-        <v>3735</v>
+        <v>3734</v>
       </c>
       <c r="B2791" s="1">
         <v>8.0299999999999994</v>
       </c>
       <c r="C2791" s="2" t="s">
-        <v>3736</v>
+        <v>3735</v>
       </c>
     </row>
     <row r="2792" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2792" s="2" t="s">
-        <v>3737</v>
+        <v>3736</v>
       </c>
       <c r="B2792" s="1">
         <v>6</v>
@@ -41013,51 +41025,51 @@
     </row>
     <row r="2793" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2793" s="2" t="s">
-        <v>3738</v>
+        <v>3737</v>
       </c>
       <c r="B2793" s="1">
         <v>9.0399999999999991</v>
       </c>
       <c r="C2793" s="2" t="s">
-        <v>3739</v>
+        <v>3738</v>
       </c>
     </row>
     <row r="2794" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2794" s="2" t="s">
-        <v>3740</v>
+        <v>3739</v>
       </c>
       <c r="B2794" s="1">
         <v>6.06</v>
       </c>
       <c r="C2794" s="2" t="s">
-        <v>3741</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="2795" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2795" s="2" t="s">
-        <v>3742</v>
+        <v>3741</v>
       </c>
       <c r="B2795" s="1">
         <v>8</v>
       </c>
       <c r="C2795" s="2" t="s">
-        <v>3743</v>
+        <v>3742</v>
       </c>
     </row>
     <row r="2796" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2796" s="2" t="s">
-        <v>3744</v>
+        <v>3743</v>
       </c>
       <c r="B2796" s="1">
         <v>9.14</v>
       </c>
       <c r="C2796" s="2" t="s">
-        <v>3745</v>
+        <v>3744</v>
       </c>
     </row>
     <row r="2797" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2797" s="2" t="s">
-        <v>3746</v>
+        <v>3745</v>
       </c>
       <c r="B2797" s="1">
         <v>6.06</v>
@@ -41068,29 +41080,29 @@
     </row>
     <row r="2798" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2798" s="2" t="s">
-        <v>3747</v>
+        <v>3746</v>
       </c>
       <c r="B2798" s="1">
         <v>6.09</v>
       </c>
       <c r="C2798" s="2" t="s">
-        <v>3748</v>
+        <v>3747</v>
       </c>
     </row>
     <row r="2799" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2799" s="2" t="s">
-        <v>3749</v>
+        <v>3748</v>
       </c>
       <c r="B2799" s="1">
         <v>10</v>
       </c>
       <c r="C2799" s="2" t="s">
-        <v>3750</v>
+        <v>3749</v>
       </c>
     </row>
     <row r="2800" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2800" s="2" t="s">
-        <v>3751</v>
+        <v>3750</v>
       </c>
       <c r="B2800" s="1">
         <v>6.25</v>
@@ -41101,51 +41113,51 @@
     </row>
     <row r="2801" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2801" s="2" t="s">
-        <v>3752</v>
+        <v>3751</v>
       </c>
       <c r="B2801" s="1">
         <v>9.25</v>
       </c>
       <c r="C2801" s="2" t="s">
-        <v>3590</v>
+        <v>3589</v>
       </c>
     </row>
     <row r="2802" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2802" s="2" t="s">
-        <v>3753</v>
+        <v>3752</v>
       </c>
       <c r="B2802" s="1">
         <v>6.52</v>
       </c>
       <c r="C2802" s="2" t="s">
-        <v>3754</v>
+        <v>3753</v>
       </c>
     </row>
     <row r="2803" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2803" s="2" t="s">
-        <v>3755</v>
+        <v>3754</v>
       </c>
       <c r="B2803" s="1">
         <v>11.11</v>
       </c>
       <c r="C2803" s="2" t="s">
-        <v>3756</v>
+        <v>3755</v>
       </c>
     </row>
     <row r="2804" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2804" s="2" t="s">
-        <v>3757</v>
+        <v>3756</v>
       </c>
       <c r="B2804" s="1">
         <v>7.35</v>
       </c>
       <c r="C2804" s="2" t="s">
-        <v>3758</v>
+        <v>3757</v>
       </c>
     </row>
     <row r="2805" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2805" s="2" t="s">
-        <v>3759</v>
+        <v>3758</v>
       </c>
       <c r="B2805" s="1">
         <v>5</v>
@@ -41156,7 +41168,7 @@
     </row>
     <row r="2806" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2806" s="2" t="s">
-        <v>3760</v>
+        <v>3759</v>
       </c>
       <c r="B2806" s="1">
         <v>7</v>
@@ -41167,7 +41179,7 @@
     </row>
     <row r="2807" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2807" s="2" t="s">
-        <v>3761</v>
+        <v>3760</v>
       </c>
       <c r="B2807" s="1">
         <v>10.07</v>
@@ -41178,7 +41190,7 @@
     </row>
     <row r="2808" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2808" s="2" t="s">
-        <v>3762</v>
+        <v>3761</v>
       </c>
       <c r="B2808" s="1">
         <v>8.01</v>
@@ -41189,18 +41201,18 @@
     </row>
     <row r="2809" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2809" s="2" t="s">
-        <v>3763</v>
+        <v>3762</v>
       </c>
       <c r="B2809" s="1">
         <v>5</v>
       </c>
       <c r="C2809" s="2" t="s">
-        <v>3764</v>
+        <v>3763</v>
       </c>
     </row>
     <row r="2810" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2810" s="2" t="s">
-        <v>3765</v>
+        <v>3764</v>
       </c>
       <c r="B2810" s="1">
         <v>5.23</v>
@@ -41211,40 +41223,40 @@
     </row>
     <row r="2811" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2811" s="2" t="s">
-        <v>3766</v>
+        <v>3765</v>
       </c>
       <c r="B2811" s="1">
         <v>6.46</v>
       </c>
       <c r="C2811" s="2" t="s">
-        <v>3767</v>
+        <v>3766</v>
       </c>
     </row>
     <row r="2812" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2812" s="2" t="s">
-        <v>3768</v>
+        <v>3767</v>
       </c>
       <c r="B2812" s="1">
         <v>7.43</v>
       </c>
       <c r="C2812" s="2" t="s">
-        <v>3769</v>
+        <v>3768</v>
       </c>
     </row>
     <row r="2813" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2813" s="2" t="s">
-        <v>3770</v>
+        <v>3769</v>
       </c>
       <c r="B2813" s="1">
         <v>7.03</v>
       </c>
       <c r="C2813" s="2" t="s">
-        <v>3771</v>
+        <v>3770</v>
       </c>
     </row>
     <row r="2814" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2814" s="2" t="s">
-        <v>3772</v>
+        <v>3771</v>
       </c>
       <c r="B2814" s="1">
         <v>12.42</v>
@@ -41255,7 +41267,7 @@
     </row>
     <row r="2815" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2815" s="2" t="s">
-        <v>3773</v>
+        <v>3772</v>
       </c>
       <c r="B2815" s="1">
         <v>3</v>
@@ -41266,7 +41278,7 @@
     </row>
     <row r="2816" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2816" s="2" t="s">
-        <v>3774</v>
+        <v>3773</v>
       </c>
       <c r="B2816" s="1">
         <v>4.0999999999999996</v>
@@ -41277,18 +41289,18 @@
     </row>
     <row r="2817" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2817" s="2" t="s">
-        <v>3775</v>
+        <v>3774</v>
       </c>
       <c r="B2817" s="1">
         <v>6.03</v>
       </c>
       <c r="C2817" s="2" t="s">
-        <v>3562</v>
+        <v>3561</v>
       </c>
     </row>
     <row r="2818" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2818" s="2" t="s">
-        <v>3776</v>
+        <v>3775</v>
       </c>
       <c r="B2818" s="1">
         <v>8</v>
@@ -41299,29 +41311,29 @@
     </row>
     <row r="2819" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2819" s="2" t="s">
-        <v>3777</v>
+        <v>3776</v>
       </c>
       <c r="B2819" s="1">
         <v>7.04</v>
       </c>
       <c r="C2819" s="2" t="s">
-        <v>3778</v>
+        <v>3777</v>
       </c>
     </row>
     <row r="2820" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2820" s="2" t="s">
-        <v>3779</v>
+        <v>3778</v>
       </c>
       <c r="B2820" s="1">
         <v>9.25</v>
       </c>
       <c r="C2820" s="2" t="s">
-        <v>3780</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="2821" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2821" s="2" t="s">
-        <v>3781</v>
+        <v>3780</v>
       </c>
       <c r="B2821" s="1">
         <v>6</v>
@@ -41332,18 +41344,18 @@
     </row>
     <row r="2822" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2822" s="2" t="s">
-        <v>3782</v>
+        <v>3781</v>
       </c>
       <c r="B2822" s="1">
         <v>7</v>
       </c>
       <c r="C2822" s="2" t="s">
-        <v>3783</v>
+        <v>3782</v>
       </c>
     </row>
     <row r="2823" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2823" s="2" t="s">
-        <v>3784</v>
+        <v>3783</v>
       </c>
       <c r="B2823" s="1">
         <v>8.0500000000000007</v>
@@ -41354,7 +41366,7 @@
     </row>
     <row r="2824" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2824" s="2" t="s">
-        <v>3785</v>
+        <v>3784</v>
       </c>
       <c r="B2824" s="1">
         <v>7.26</v>
@@ -41365,51 +41377,51 @@
     </row>
     <row r="2825" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2825" s="2" t="s">
-        <v>3786</v>
+        <v>3785</v>
       </c>
       <c r="B2825" s="1">
         <v>13.1</v>
       </c>
       <c r="C2825" s="2" t="s">
-        <v>3787</v>
+        <v>3786</v>
       </c>
     </row>
     <row r="2826" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2826" s="2" t="s">
-        <v>3788</v>
+        <v>3787</v>
       </c>
       <c r="B2826" s="1">
         <v>8.07</v>
       </c>
       <c r="C2826" s="2" t="s">
-        <v>3789</v>
+        <v>3788</v>
       </c>
     </row>
     <row r="2827" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2827" s="2" t="s">
-        <v>3790</v>
+        <v>3789</v>
       </c>
       <c r="B2827" s="1">
         <v>10</v>
       </c>
       <c r="C2827" s="2" t="s">
-        <v>3791</v>
+        <v>3790</v>
       </c>
     </row>
     <row r="2828" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2828" s="2" t="s">
-        <v>3792</v>
+        <v>3791</v>
       </c>
       <c r="B2828" s="1">
         <v>9.14</v>
       </c>
       <c r="C2828" s="2" t="s">
-        <v>3789</v>
+        <v>3788</v>
       </c>
     </row>
     <row r="2829" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2829" s="2" t="s">
-        <v>3793</v>
+        <v>3792</v>
       </c>
       <c r="B2829" s="1">
         <v>7</v>
@@ -41420,62 +41432,62 @@
     </row>
     <row r="2830" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2830" s="2" t="s">
-        <v>3794</v>
+        <v>3793</v>
       </c>
       <c r="B2830" s="1">
         <v>4.01</v>
       </c>
       <c r="C2830" s="2" t="s">
-        <v>3795</v>
+        <v>3794</v>
       </c>
     </row>
     <row r="2831" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2831" s="2" t="s">
-        <v>3796</v>
+        <v>3795</v>
       </c>
       <c r="B2831" s="1">
         <v>6.36</v>
       </c>
       <c r="C2831" s="2" t="s">
-        <v>3797</v>
+        <v>3796</v>
       </c>
     </row>
     <row r="2832" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2832" s="2" t="s">
-        <v>3798</v>
+        <v>3797</v>
       </c>
       <c r="B2832" s="1">
         <v>6.13</v>
       </c>
       <c r="C2832" s="2" t="s">
-        <v>3799</v>
+        <v>3798</v>
       </c>
     </row>
     <row r="2833" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2833" s="2" t="s">
-        <v>3800</v>
+        <v>3799</v>
       </c>
       <c r="B2833" s="1">
         <v>6</v>
       </c>
       <c r="C2833" s="2" t="s">
-        <v>3801</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="2834" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2834" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="B2834" s="1">
         <v>1.58</v>
       </c>
       <c r="C2834" s="2" t="s">
-        <v>3803</v>
+        <v>3802</v>
       </c>
     </row>
     <row r="2835" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2835" s="2" t="s">
-        <v>3802</v>
+        <v>3801</v>
       </c>
       <c r="B2835" s="1">
         <v>4.5</v>
@@ -41483,84 +41495,84 @@
     </row>
     <row r="2836" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2836" s="2" t="s">
-        <v>3804</v>
+        <v>3803</v>
       </c>
       <c r="B2836" s="1">
         <v>10</v>
       </c>
       <c r="C2836" s="2" t="s">
-        <v>3805</v>
+        <v>3804</v>
       </c>
     </row>
     <row r="2837" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2837" s="2" t="s">
-        <v>3806</v>
+        <v>3805</v>
       </c>
       <c r="B2837" s="1">
         <v>7</v>
       </c>
       <c r="C2837" s="2" t="s">
-        <v>3807</v>
+        <v>3806</v>
       </c>
     </row>
     <row r="2838" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2838" s="2" t="s">
-        <v>3808</v>
+        <v>3807</v>
       </c>
       <c r="B2838" s="1">
         <v>7.18</v>
       </c>
       <c r="C2838" s="2" t="s">
-        <v>3809</v>
+        <v>3808</v>
       </c>
     </row>
     <row r="2839" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2839" s="2" t="s">
-        <v>3810</v>
+        <v>3809</v>
       </c>
       <c r="B2839" s="1">
         <v>7.04</v>
       </c>
       <c r="C2839" s="2" t="s">
-        <v>3811</v>
+        <v>3810</v>
       </c>
     </row>
     <row r="2840" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2840" s="2" t="s">
-        <v>3812</v>
+        <v>3811</v>
       </c>
       <c r="B2840" s="1">
         <v>4</v>
       </c>
       <c r="C2840" s="2" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
     </row>
     <row r="2841" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2841" s="2" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B2841" s="1">
         <v>6</v>
       </c>
       <c r="C2841" s="2" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
     </row>
     <row r="2842" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2842" s="2" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="B2842" s="1">
         <v>9.07</v>
       </c>
       <c r="C2842" s="2" t="s">
-        <v>3817</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="2843" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2843" s="2" t="s">
-        <v>3818</v>
+        <v>3817</v>
       </c>
       <c r="B2843" s="1">
         <v>6.01</v>
@@ -41571,18 +41583,18 @@
     </row>
     <row r="2844" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2844" s="2" t="s">
-        <v>3819</v>
+        <v>3818</v>
       </c>
       <c r="B2844" s="1">
         <v>6</v>
       </c>
       <c r="C2844" s="2" t="s">
-        <v>3820</v>
+        <v>3819</v>
       </c>
     </row>
     <row r="2845" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2845" s="2" t="s">
-        <v>3821</v>
+        <v>3820</v>
       </c>
       <c r="B2845" s="1">
         <v>8.4600000000000009</v>
@@ -41593,29 +41605,29 @@
     </row>
     <row r="2846" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2846" s="2" t="s">
-        <v>3822</v>
+        <v>3821</v>
       </c>
       <c r="B2846" s="1">
         <v>12.09</v>
       </c>
       <c r="C2846" s="2" t="s">
-        <v>3823</v>
+        <v>3822</v>
       </c>
     </row>
     <row r="2847" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2847" s="2" t="s">
-        <v>3824</v>
+        <v>3823</v>
       </c>
       <c r="B2847" s="1">
         <v>8</v>
       </c>
       <c r="C2847" s="2" t="s">
-        <v>3825</v>
+        <v>3824</v>
       </c>
     </row>
     <row r="2848" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2848" s="2" t="s">
-        <v>3826</v>
+        <v>3825</v>
       </c>
       <c r="B2848" s="1">
         <v>9.07</v>
@@ -41626,7 +41638,7 @@
     </row>
     <row r="2849" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2849" s="2" t="s">
-        <v>3827</v>
+        <v>3826</v>
       </c>
       <c r="B2849" s="1">
         <v>6.32</v>
@@ -41637,51 +41649,51 @@
     </row>
     <row r="2850" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2850" s="2" t="s">
-        <v>3828</v>
+        <v>3827</v>
       </c>
       <c r="B2850" s="1">
         <v>9.0399999999999991</v>
       </c>
       <c r="C2850" s="2" t="s">
-        <v>3829</v>
+        <v>3828</v>
       </c>
     </row>
     <row r="2851" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2851" s="2" t="s">
-        <v>3830</v>
+        <v>3829</v>
       </c>
       <c r="B2851" s="1">
         <v>13.11</v>
       </c>
       <c r="C2851" s="2" t="s">
-        <v>3831</v>
+        <v>3830</v>
       </c>
     </row>
     <row r="2852" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2852" s="2" t="s">
-        <v>3832</v>
+        <v>3831</v>
       </c>
       <c r="B2852" s="1">
         <v>10</v>
       </c>
       <c r="C2852" s="2" t="s">
-        <v>3833</v>
+        <v>3832</v>
       </c>
     </row>
     <row r="2853" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2853" s="2" t="s">
-        <v>3834</v>
+        <v>3833</v>
       </c>
       <c r="B2853" s="1">
         <v>6.01</v>
       </c>
       <c r="C2853" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
     </row>
     <row r="2854" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2854" s="2" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="B2854" s="1">
         <v>9.1</v>
@@ -41692,18 +41704,18 @@
     </row>
     <row r="2855" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2855" s="2" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="B2855" s="1">
         <v>6</v>
       </c>
       <c r="C2855" s="2" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
     </row>
     <row r="2856" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2856" s="2" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="B2856" s="1">
         <v>6.04</v>
@@ -41714,29 +41726,29 @@
     </row>
     <row r="2857" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2857" s="2" t="s">
-        <v>3840</v>
+        <v>3839</v>
       </c>
       <c r="B2857" s="1">
         <v>14</v>
       </c>
       <c r="C2857" s="2" t="s">
-        <v>3841</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="2858" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2858" s="2" t="s">
-        <v>3842</v>
+        <v>3841</v>
       </c>
       <c r="B2858" s="1">
         <v>10</v>
       </c>
       <c r="C2858" s="2" t="s">
-        <v>3843</v>
+        <v>3842</v>
       </c>
     </row>
     <row r="2859" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2859" s="2" t="s">
-        <v>3844</v>
+        <v>3843</v>
       </c>
       <c r="B2859" s="1">
         <v>8</v>
@@ -41747,29 +41759,29 @@
     </row>
     <row r="2860" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2860" s="2" t="s">
-        <v>3845</v>
+        <v>3844</v>
       </c>
       <c r="B2860" s="1">
         <v>10</v>
       </c>
       <c r="C2860" s="2" t="s">
-        <v>3846</v>
+        <v>3845</v>
       </c>
     </row>
     <row r="2861" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2861" s="2" t="s">
-        <v>3847</v>
+        <v>3846</v>
       </c>
       <c r="B2861" s="1">
         <v>6</v>
       </c>
       <c r="C2861" s="2" t="s">
-        <v>3848</v>
+        <v>3847</v>
       </c>
     </row>
     <row r="2862" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2862" s="2" t="s">
-        <v>3849</v>
+        <v>3848</v>
       </c>
       <c r="B2862" s="1">
         <v>7.83</v>
@@ -41780,18 +41792,18 @@
     </row>
     <row r="2863" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2863" s="2" t="s">
-        <v>3850</v>
+        <v>3849</v>
       </c>
       <c r="B2863" s="1">
         <v>3.11</v>
       </c>
       <c r="C2863" s="2" t="s">
-        <v>3851</v>
+        <v>3850</v>
       </c>
     </row>
     <row r="2864" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2864" s="2" t="s">
-        <v>3850</v>
+        <v>3849</v>
       </c>
       <c r="B2864" s="1">
         <v>5.4</v>
@@ -41799,40 +41811,40 @@
     </row>
     <row r="2865" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2865" s="2" t="s">
-        <v>3852</v>
+        <v>3851</v>
       </c>
       <c r="B2865" s="1">
         <v>10.050000000000001</v>
       </c>
       <c r="C2865" s="2" t="s">
-        <v>3853</v>
+        <v>3852</v>
       </c>
     </row>
     <row r="2866" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2866" s="2" t="s">
-        <v>3854</v>
+        <v>3853</v>
       </c>
       <c r="B2866" s="1">
         <v>6</v>
       </c>
       <c r="C2866" s="2" t="s">
-        <v>3855</v>
+        <v>3854</v>
       </c>
     </row>
     <row r="2867" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2867" s="2" t="s">
-        <v>3856</v>
+        <v>3855</v>
       </c>
       <c r="B2867" s="1">
         <v>10</v>
       </c>
       <c r="C2867" s="2" t="s">
-        <v>3857</v>
+        <v>3856</v>
       </c>
     </row>
     <row r="2868" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2868" s="2" t="s">
-        <v>3858</v>
+        <v>3857</v>
       </c>
       <c r="B2868" s="1">
         <v>6.02</v>
@@ -41843,7 +41855,7 @@
     </row>
     <row r="2869" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2869" s="2" t="s">
-        <v>3859</v>
+        <v>3858</v>
       </c>
       <c r="B2869" s="1">
         <v>4.01</v>
@@ -41854,29 +41866,29 @@
     </row>
     <row r="2870" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2870" s="2" t="s">
-        <v>3860</v>
+        <v>3859</v>
       </c>
       <c r="B2870" s="1">
         <v>8.0399999999999991</v>
       </c>
       <c r="C2870" s="2" t="s">
-        <v>3861</v>
+        <v>3860</v>
       </c>
     </row>
     <row r="2871" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2871" s="2" t="s">
-        <v>3862</v>
+        <v>3861</v>
       </c>
       <c r="B2871" s="1">
         <v>13.1</v>
       </c>
       <c r="C2871" s="2" t="s">
-        <v>3863</v>
+        <v>3862</v>
       </c>
     </row>
     <row r="2872" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2872" s="2" t="s">
-        <v>3864</v>
+        <v>3863</v>
       </c>
       <c r="B2872" s="1">
         <v>5.7</v>
@@ -41887,18 +41899,18 @@
     </row>
     <row r="2873" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2873" s="2" t="s">
-        <v>3865</v>
+        <v>3864</v>
       </c>
       <c r="B2873" s="1">
         <v>6.34</v>
       </c>
       <c r="C2873" s="2" t="s">
-        <v>3866</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="2874" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2874" s="2" t="s">
-        <v>3867</v>
+        <v>3866</v>
       </c>
       <c r="B2874" s="1">
         <v>7.03</v>
@@ -41909,29 +41921,29 @@
     </row>
     <row r="2875" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2875" s="2" t="s">
-        <v>3868</v>
+        <v>3867</v>
       </c>
       <c r="B2875" s="1">
         <v>4.04</v>
       </c>
       <c r="C2875" s="2" t="s">
-        <v>3869</v>
+        <v>3868</v>
       </c>
     </row>
     <row r="2876" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2876" s="2" t="s">
-        <v>3870</v>
+        <v>3869</v>
       </c>
       <c r="B2876" s="1">
         <v>6</v>
       </c>
       <c r="C2876" s="2" t="s">
-        <v>3871</v>
+        <v>3870</v>
       </c>
     </row>
     <row r="2877" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2877" s="2" t="s">
-        <v>3872</v>
+        <v>3871</v>
       </c>
       <c r="B2877" s="1">
         <v>4.01</v>
@@ -41942,18 +41954,18 @@
     </row>
     <row r="2878" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2878" s="2" t="s">
-        <v>3873</v>
+        <v>3872</v>
       </c>
       <c r="B2878" s="1">
         <v>13.11</v>
       </c>
       <c r="C2878" s="2" t="s">
-        <v>3874</v>
+        <v>3873</v>
       </c>
     </row>
     <row r="2879" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2879" s="2" t="s">
-        <v>3873</v>
+        <v>3872</v>
       </c>
       <c r="B2879" s="1">
         <v>3</v>
@@ -41961,29 +41973,29 @@
     </row>
     <row r="2880" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2880" s="2" t="s">
-        <v>3875</v>
+        <v>3874</v>
       </c>
       <c r="B2880" s="1">
         <v>3.76</v>
       </c>
       <c r="C2880" s="2" t="s">
-        <v>3876</v>
+        <v>3875</v>
       </c>
     </row>
     <row r="2881" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2881" s="2" t="s">
-        <v>3877</v>
+        <v>3876</v>
       </c>
       <c r="B2881" s="1">
         <v>5.2</v>
       </c>
       <c r="C2881" s="2" t="s">
-        <v>3878</v>
+        <v>3877</v>
       </c>
     </row>
     <row r="2882" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2882" s="2" t="s">
-        <v>3879</v>
+        <v>3878</v>
       </c>
       <c r="B2882" s="1">
         <v>6.3</v>
@@ -41994,13 +42006,35 @@
     </row>
     <row r="2883" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2883" s="2" t="s">
-        <v>3880</v>
+        <v>3879</v>
       </c>
       <c r="B2883" s="1">
         <v>4.0599999999999996</v>
       </c>
       <c r="C2883" s="2" t="s">
+        <v>3880</v>
+      </c>
+    </row>
+    <row r="2884" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2884" s="2" t="s">
         <v>3881</v>
+      </c>
+      <c r="B2884" s="1">
+        <v>7.04</v>
+      </c>
+      <c r="C2884" s="2" t="s">
+        <v>3882</v>
+      </c>
+    </row>
+    <row r="2885" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2885" s="2" t="s">
+        <v>3883</v>
+      </c>
+      <c r="B2885" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2885" s="2" t="s">
+        <v>3884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first update in a while 30nov2022
</commit_message>
<xml_diff>
--- a/Running_Log.xlsx
+++ b/Running_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlexDolwick/dolwick_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE435137-E6B6-414A-9B8A-1E414DCC483B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC9A6F-00E9-5D43-9142-EE58E01E587C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="460" windowWidth="25680" windowHeight="15920" xr2:uid="{4B2E00A5-7125-EC4E-9EAD-C4CEE86B127A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4693" uniqueCount="3933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4898" uniqueCount="4093">
   <si>
     <t>Date</t>
   </si>
@@ -11832,6 +11832,486 @@
   </si>
   <si>
     <t>2009-01-05</t>
+  </si>
+  <si>
+    <t>2022-01-05</t>
+  </si>
+  <si>
+    <t>2022-01-06</t>
+  </si>
+  <si>
+    <t>2022-01-10</t>
+  </si>
+  <si>
+    <t>28:40</t>
+  </si>
+  <si>
+    <t>2022-01-12</t>
+  </si>
+  <si>
+    <t>2022-01-19</t>
+  </si>
+  <si>
+    <t>29:10</t>
+  </si>
+  <si>
+    <t>2022-01-22</t>
+  </si>
+  <si>
+    <t>23:53</t>
+  </si>
+  <si>
+    <t>2022-01-25</t>
+  </si>
+  <si>
+    <t>27:16</t>
+  </si>
+  <si>
+    <t>2022-02-25</t>
+  </si>
+  <si>
+    <t>2022-03-06</t>
+  </si>
+  <si>
+    <t>32:58</t>
+  </si>
+  <si>
+    <t>2022-03-10</t>
+  </si>
+  <si>
+    <t>34:37</t>
+  </si>
+  <si>
+    <t>2022-03-14</t>
+  </si>
+  <si>
+    <t>35:21</t>
+  </si>
+  <si>
+    <t>2022-03-17</t>
+  </si>
+  <si>
+    <t>41:06</t>
+  </si>
+  <si>
+    <t>2022-03-22</t>
+  </si>
+  <si>
+    <t>2022-03-26</t>
+  </si>
+  <si>
+    <t>40:27</t>
+  </si>
+  <si>
+    <t>2022-04-04</t>
+  </si>
+  <si>
+    <t>2022-04-06</t>
+  </si>
+  <si>
+    <t>30:26</t>
+  </si>
+  <si>
+    <t>2022-04-09</t>
+  </si>
+  <si>
+    <t>36:20</t>
+  </si>
+  <si>
+    <t>2022-04-11</t>
+  </si>
+  <si>
+    <t>2022-04-16</t>
+  </si>
+  <si>
+    <t>2022-04-22</t>
+  </si>
+  <si>
+    <t>29:47</t>
+  </si>
+  <si>
+    <t>2022-04-25</t>
+  </si>
+  <si>
+    <t>34:35</t>
+  </si>
+  <si>
+    <t>2022-04-28</t>
+  </si>
+  <si>
+    <t>42:29</t>
+  </si>
+  <si>
+    <t>2022-05-01</t>
+  </si>
+  <si>
+    <t>2022-05-05</t>
+  </si>
+  <si>
+    <t>2022-05-08</t>
+  </si>
+  <si>
+    <t>39:47</t>
+  </si>
+  <si>
+    <t>2022-05-11</t>
+  </si>
+  <si>
+    <t>2022-05-18</t>
+  </si>
+  <si>
+    <t>43:03</t>
+  </si>
+  <si>
+    <t>2022-05-24</t>
+  </si>
+  <si>
+    <t>2022-05-26</t>
+  </si>
+  <si>
+    <t>2022-06-03</t>
+  </si>
+  <si>
+    <t>35:08</t>
+  </si>
+  <si>
+    <t>2022-06-07</t>
+  </si>
+  <si>
+    <t>2022-06-14</t>
+  </si>
+  <si>
+    <t>29:43</t>
+  </si>
+  <si>
+    <t>2022-06-16</t>
+  </si>
+  <si>
+    <t>2022-07-02</t>
+  </si>
+  <si>
+    <t>2022-07-04</t>
+  </si>
+  <si>
+    <t>32:37</t>
+  </si>
+  <si>
+    <t>2022-07-14</t>
+  </si>
+  <si>
+    <t>2022-07-22</t>
+  </si>
+  <si>
+    <t>36:28</t>
+  </si>
+  <si>
+    <t>2022-07-25</t>
+  </si>
+  <si>
+    <t>2022-07-29</t>
+  </si>
+  <si>
+    <t>39:23</t>
+  </si>
+  <si>
+    <t>2022-07-31</t>
+  </si>
+  <si>
+    <t>23:10</t>
+  </si>
+  <si>
+    <t>2022-08-03</t>
+  </si>
+  <si>
+    <t>19:49</t>
+  </si>
+  <si>
+    <t>2022-08-07</t>
+  </si>
+  <si>
+    <t>41:35</t>
+  </si>
+  <si>
+    <t>2022-08-10</t>
+  </si>
+  <si>
+    <t>48:27</t>
+  </si>
+  <si>
+    <t>2022-08-12</t>
+  </si>
+  <si>
+    <t>49:25</t>
+  </si>
+  <si>
+    <t>2022-08-14</t>
+  </si>
+  <si>
+    <t>2022-08-17</t>
+  </si>
+  <si>
+    <t>2022-08-19</t>
+  </si>
+  <si>
+    <t>2022-08-22</t>
+  </si>
+  <si>
+    <t>35:44</t>
+  </si>
+  <si>
+    <t>2022-08-24</t>
+  </si>
+  <si>
+    <t>2022-08-26</t>
+  </si>
+  <si>
+    <t>2022-08-29</t>
+  </si>
+  <si>
+    <t>2022-08-31</t>
+  </si>
+  <si>
+    <t>56:29</t>
+  </si>
+  <si>
+    <t>2022-09-02</t>
+  </si>
+  <si>
+    <t>24:27</t>
+  </si>
+  <si>
+    <t>2022-09-04</t>
+  </si>
+  <si>
+    <t>2022-09-06</t>
+  </si>
+  <si>
+    <t>30:41</t>
+  </si>
+  <si>
+    <t>2022-09-07</t>
+  </si>
+  <si>
+    <t>48:29</t>
+  </si>
+  <si>
+    <t>2022-09-09</t>
+  </si>
+  <si>
+    <t>2022-09-11</t>
+  </si>
+  <si>
+    <t>1:03:49</t>
+  </si>
+  <si>
+    <t>2022-09-12</t>
+  </si>
+  <si>
+    <t>34:42</t>
+  </si>
+  <si>
+    <t>2022-09-14</t>
+  </si>
+  <si>
+    <t>1:06:59</t>
+  </si>
+  <si>
+    <t>2022-09-16</t>
+  </si>
+  <si>
+    <t>49:19</t>
+  </si>
+  <si>
+    <t>2022-09-17</t>
+  </si>
+  <si>
+    <t>2022-09-19</t>
+  </si>
+  <si>
+    <t>48:59</t>
+  </si>
+  <si>
+    <t>2022-09-21</t>
+  </si>
+  <si>
+    <t>2022-09-23</t>
+  </si>
+  <si>
+    <t>38:08</t>
+  </si>
+  <si>
+    <t>2022-09-24</t>
+  </si>
+  <si>
+    <t>2022-09-26</t>
+  </si>
+  <si>
+    <t>2022-09-28</t>
+  </si>
+  <si>
+    <t>1:05:22</t>
+  </si>
+  <si>
+    <t>2022-09-30</t>
+  </si>
+  <si>
+    <t>31:55</t>
+  </si>
+  <si>
+    <t>2022-10-01</t>
+  </si>
+  <si>
+    <t>2022-10-03</t>
+  </si>
+  <si>
+    <t>2022-10-05</t>
+  </si>
+  <si>
+    <t>1:07:41</t>
+  </si>
+  <si>
+    <t>2022-10-07</t>
+  </si>
+  <si>
+    <t>28:38</t>
+  </si>
+  <si>
+    <t>2022-10-09</t>
+  </si>
+  <si>
+    <t>2022-10-10</t>
+  </si>
+  <si>
+    <t>50:42</t>
+  </si>
+  <si>
+    <t>2022-10-12</t>
+  </si>
+  <si>
+    <t>1:23:24</t>
+  </si>
+  <si>
+    <t>2022-10-14</t>
+  </si>
+  <si>
+    <t>2022-10-15</t>
+  </si>
+  <si>
+    <t>29:16</t>
+  </si>
+  <si>
+    <t>2022-10-17</t>
+  </si>
+  <si>
+    <t>43:30</t>
+  </si>
+  <si>
+    <t>2022-10-19</t>
+  </si>
+  <si>
+    <t>54:30</t>
+  </si>
+  <si>
+    <t>2022-10-20</t>
+  </si>
+  <si>
+    <t>1:24:39</t>
+  </si>
+  <si>
+    <t>2022-10-23</t>
+  </si>
+  <si>
+    <t>2022-10-24</t>
+  </si>
+  <si>
+    <t>1:02:05</t>
+  </si>
+  <si>
+    <t>2022-10-26</t>
+  </si>
+  <si>
+    <t>1:11:54</t>
+  </si>
+  <si>
+    <t>2022-10-29</t>
+  </si>
+  <si>
+    <t>1:22:14</t>
+  </si>
+  <si>
+    <t>2022-10-31</t>
+  </si>
+  <si>
+    <t>46:09</t>
+  </si>
+  <si>
+    <t>2022-11-02</t>
+  </si>
+  <si>
+    <t>55:46</t>
+  </si>
+  <si>
+    <t>2022-11-04</t>
+  </si>
+  <si>
+    <t>2022-11-06</t>
+  </si>
+  <si>
+    <t>1:18:11</t>
+  </si>
+  <si>
+    <t>2022-11-08</t>
+  </si>
+  <si>
+    <t>58:45</t>
+  </si>
+  <si>
+    <t>2022-11-09</t>
+  </si>
+  <si>
+    <t>1:01:02</t>
+  </si>
+  <si>
+    <t>2022-11-11</t>
+  </si>
+  <si>
+    <t>2022-11-13</t>
+  </si>
+  <si>
+    <t>1:23:55</t>
+  </si>
+  <si>
+    <t>2022-11-16</t>
+  </si>
+  <si>
+    <t>38:57</t>
+  </si>
+  <si>
+    <t>2022-11-18</t>
+  </si>
+  <si>
+    <t>2022-11-19</t>
+  </si>
+  <si>
+    <t>17:08</t>
+  </si>
+  <si>
+    <t>2022-11-21</t>
+  </si>
+  <si>
+    <t>2022-11-23</t>
+  </si>
+  <si>
+    <t>1:01:59</t>
+  </si>
+  <si>
+    <t>2022-11-24</t>
+  </si>
+  <si>
+    <t>2022-11-26</t>
+  </si>
+  <si>
+    <t>2022-11-29</t>
   </si>
 </sst>
 </file>
@@ -12208,10 +12688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BECE25-7878-7543-A5E4-1B4438F2AAC2}">
-  <dimension ref="A1:E2920"/>
+  <dimension ref="A1:E3024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2904" workbookViewId="0">
-      <selection activeCell="C2924" sqref="C2924"/>
+    <sheetView tabSelected="1" topLeftCell="A3000" workbookViewId="0">
+      <selection activeCell="B3025" sqref="B3025"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42564,6 +43044,1141 @@
         <v>2448</v>
       </c>
     </row>
+    <row r="2921" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2921" s="2" t="s">
+        <v>3933</v>
+      </c>
+      <c r="B2921" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C2921" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2922" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2922" s="2" t="s">
+        <v>3934</v>
+      </c>
+      <c r="B2922" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2922" s="2" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="2923" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2923" s="2" t="s">
+        <v>3935</v>
+      </c>
+      <c r="B2923" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="C2923" s="2" t="s">
+        <v>3936</v>
+      </c>
+    </row>
+    <row r="2924" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2924" s="2" t="s">
+        <v>3937</v>
+      </c>
+      <c r="B2924" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2924" s="2" t="s">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="2925" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2925" s="2" t="s">
+        <v>3938</v>
+      </c>
+      <c r="B2925" s="1">
+        <v>4.03</v>
+      </c>
+      <c r="C2925" s="2" t="s">
+        <v>3939</v>
+      </c>
+    </row>
+    <row r="2926" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2926" s="2" t="s">
+        <v>3940</v>
+      </c>
+      <c r="B2926" s="1">
+        <v>3.16</v>
+      </c>
+      <c r="C2926" s="2" t="s">
+        <v>3941</v>
+      </c>
+    </row>
+    <row r="2927" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2927" s="2" t="s">
+        <v>3942</v>
+      </c>
+      <c r="B2927" s="1">
+        <v>4.07</v>
+      </c>
+      <c r="C2927" s="2" t="s">
+        <v>3943</v>
+      </c>
+    </row>
+    <row r="2928" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2928" s="2" t="s">
+        <v>3944</v>
+      </c>
+      <c r="B2928" s="1">
+        <v>3.45</v>
+      </c>
+      <c r="C2928" s="2" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="2929" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2929" s="2" t="s">
+        <v>3945</v>
+      </c>
+      <c r="B2929" s="1">
+        <v>4.38</v>
+      </c>
+      <c r="C2929" s="2" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="2930" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2930" s="2" t="s">
+        <v>3947</v>
+      </c>
+      <c r="B2930" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="C2930" s="2" t="s">
+        <v>3948</v>
+      </c>
+    </row>
+    <row r="2931" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2931" s="2" t="s">
+        <v>3949</v>
+      </c>
+      <c r="B2931" s="1">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="C2931" s="2" t="s">
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="2932" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2932" s="2" t="s">
+        <v>3951</v>
+      </c>
+      <c r="B2932" s="1">
+        <v>5.55</v>
+      </c>
+      <c r="C2932" s="2" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="2933" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2933" s="2" t="s">
+        <v>3953</v>
+      </c>
+      <c r="B2933" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="C2933" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2934" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2934" s="2" t="s">
+        <v>3954</v>
+      </c>
+      <c r="B2934" s="1">
+        <v>5.03</v>
+      </c>
+      <c r="C2934" s="2" t="s">
+        <v>3955</v>
+      </c>
+    </row>
+    <row r="2935" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2935" s="2" t="s">
+        <v>3956</v>
+      </c>
+      <c r="B2935" s="1">
+        <v>3.11</v>
+      </c>
+      <c r="C2935" s="2" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="2936" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2936" s="2" t="s">
+        <v>3957</v>
+      </c>
+      <c r="B2936" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C2936" s="2" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="2937" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2937" s="2" t="s">
+        <v>3959</v>
+      </c>
+      <c r="B2937" s="1">
+        <v>5.29</v>
+      </c>
+      <c r="C2937" s="2" t="s">
+        <v>3960</v>
+      </c>
+    </row>
+    <row r="2938" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2938" s="2" t="s">
+        <v>3961</v>
+      </c>
+      <c r="B2938" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C2938" s="2" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="2939" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2939" s="2" t="s">
+        <v>3962</v>
+      </c>
+      <c r="B2939" s="1">
+        <v>6.16</v>
+      </c>
+      <c r="C2939" s="2" t="s">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="2940" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2940" s="2" t="s">
+        <v>3963</v>
+      </c>
+      <c r="B2940" s="1">
+        <v>4.01</v>
+      </c>
+      <c r="C2940" s="2" t="s">
+        <v>3964</v>
+      </c>
+    </row>
+    <row r="2941" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2941" s="2" t="s">
+        <v>3965</v>
+      </c>
+      <c r="B2941" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2941" s="2" t="s">
+        <v>3966</v>
+      </c>
+    </row>
+    <row r="2942" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2942" s="2" t="s">
+        <v>3967</v>
+      </c>
+      <c r="B2942" s="1">
+        <v>6.07</v>
+      </c>
+      <c r="C2942" s="2" t="s">
+        <v>3968</v>
+      </c>
+    </row>
+    <row r="2943" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2943" s="2" t="s">
+        <v>3969</v>
+      </c>
+      <c r="B2943" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="C2943" s="2" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="2944" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2944" s="2" t="s">
+        <v>3970</v>
+      </c>
+      <c r="B2944" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2944" s="2" t="s">
+        <v>3410</v>
+      </c>
+    </row>
+    <row r="2945" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2945" s="2" t="s">
+        <v>3971</v>
+      </c>
+      <c r="B2945" s="1">
+        <v>5.55</v>
+      </c>
+      <c r="C2945" s="2" t="s">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="2946" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2946" s="2" t="s">
+        <v>3973</v>
+      </c>
+      <c r="B2946" s="1">
+        <v>4.18</v>
+      </c>
+      <c r="C2946" s="2" t="s">
+        <v>3964</v>
+      </c>
+    </row>
+    <row r="2947" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2947" s="2" t="s">
+        <v>3974</v>
+      </c>
+      <c r="B2947" s="1">
+        <v>6.11</v>
+      </c>
+      <c r="C2947" s="2" t="s">
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="2948" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2948" s="2" t="s">
+        <v>3976</v>
+      </c>
+      <c r="B2948" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C2948" s="2" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="2949" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2949" s="2" t="s">
+        <v>3977</v>
+      </c>
+      <c r="B2949" s="1">
+        <v>4.93</v>
+      </c>
+      <c r="C2949" s="2" t="s">
+        <v>3894</v>
+      </c>
+    </row>
+    <row r="2950" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2950" s="2" t="s">
+        <v>3978</v>
+      </c>
+      <c r="B2950" s="1">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="C2950" s="2" t="s">
+        <v>3979</v>
+      </c>
+    </row>
+    <row r="2951" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2951" s="2" t="s">
+        <v>3980</v>
+      </c>
+      <c r="B2951" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="C2951" s="2" t="s">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="2952" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2952" s="2" t="s">
+        <v>3981</v>
+      </c>
+      <c r="B2952" s="1">
+        <v>4.07</v>
+      </c>
+      <c r="C2952" s="2" t="s">
+        <v>3982</v>
+      </c>
+    </row>
+    <row r="2953" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2953" s="2" t="s">
+        <v>3983</v>
+      </c>
+      <c r="B2953" s="1">
+        <v>4.34</v>
+      </c>
+      <c r="C2953" s="2" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="2954" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2954" s="2" t="s">
+        <v>3984</v>
+      </c>
+      <c r="B2954" s="1">
+        <v>3.11</v>
+      </c>
+      <c r="C2954" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2955" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2955" s="2" t="s">
+        <v>3985</v>
+      </c>
+      <c r="B2955" s="1">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="C2955" s="2" t="s">
+        <v>3986</v>
+      </c>
+    </row>
+    <row r="2956" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2956" s="2" t="s">
+        <v>3987</v>
+      </c>
+      <c r="B2956" s="1">
+        <v>4.03</v>
+      </c>
+      <c r="C2956" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="2957" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2957" s="2" t="s">
+        <v>3988</v>
+      </c>
+      <c r="B2957" s="1">
+        <v>5.03</v>
+      </c>
+      <c r="C2957" s="2" t="s">
+        <v>3989</v>
+      </c>
+    </row>
+    <row r="2958" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2958" s="2" t="s">
+        <v>3990</v>
+      </c>
+      <c r="B2958" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="C2958" s="2" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="2959" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2959" s="2" t="s">
+        <v>3991</v>
+      </c>
+      <c r="B2959" s="1">
+        <v>5.29</v>
+      </c>
+      <c r="C2959" s="2" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="2960" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2960" s="2" t="s">
+        <v>3993</v>
+      </c>
+      <c r="B2960" s="1">
+        <v>3.15</v>
+      </c>
+      <c r="C2960" s="2" t="s">
+        <v>3994</v>
+      </c>
+    </row>
+    <row r="2961" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2961" s="2" t="s">
+        <v>3995</v>
+      </c>
+      <c r="B2961" s="1">
+        <v>3.11</v>
+      </c>
+      <c r="C2961" s="2" t="s">
+        <v>3996</v>
+      </c>
+    </row>
+    <row r="2962" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2962" s="2" t="s">
+        <v>3995</v>
+      </c>
+      <c r="B2962" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="2963" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2963" s="2" t="s">
+        <v>3997</v>
+      </c>
+      <c r="B2963" s="1">
+        <v>5.13</v>
+      </c>
+      <c r="C2963" s="2" t="s">
+        <v>3998</v>
+      </c>
+    </row>
+    <row r="2964" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2964" s="2" t="s">
+        <v>3999</v>
+      </c>
+      <c r="B2964" s="1">
+        <v>6.11</v>
+      </c>
+      <c r="C2964" s="2" t="s">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="2965" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2965" s="2" t="s">
+        <v>4001</v>
+      </c>
+      <c r="B2965" s="1">
+        <v>5.86</v>
+      </c>
+      <c r="C2965" s="2" t="s">
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="2966" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2966" s="2" t="s">
+        <v>4003</v>
+      </c>
+      <c r="B2966" s="1">
+        <v>5.22</v>
+      </c>
+      <c r="C2966" s="2" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="2967" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2967" s="2" t="s">
+        <v>4004</v>
+      </c>
+      <c r="B2967" s="1">
+        <v>6.04</v>
+      </c>
+      <c r="C2967" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="2968" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2968" s="2" t="s">
+        <v>4005</v>
+      </c>
+      <c r="B2968" s="1">
+        <v>5.18</v>
+      </c>
+      <c r="C2968" s="2" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="2969" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2969" s="2" t="s">
+        <v>4006</v>
+      </c>
+      <c r="B2969" s="1">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="C2969" s="2" t="s">
+        <v>4007</v>
+      </c>
+    </row>
+    <row r="2970" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2970" s="2" t="s">
+        <v>4008</v>
+      </c>
+      <c r="B2970" s="1">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="C2970" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2971" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2971" s="2" t="s">
+        <v>4009</v>
+      </c>
+      <c r="B2971" s="1">
+        <v>6.22</v>
+      </c>
+      <c r="C2971" s="2" t="s">
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="2972" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2972" s="2" t="s">
+        <v>4010</v>
+      </c>
+      <c r="B2972" s="1">
+        <v>5.88</v>
+      </c>
+      <c r="C2972" s="2" t="s">
+        <v>3796</v>
+      </c>
+    </row>
+    <row r="2973" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2973" s="2" t="s">
+        <v>4011</v>
+      </c>
+      <c r="B2973" s="1">
+        <v>7.21</v>
+      </c>
+      <c r="C2973" s="2" t="s">
+        <v>4012</v>
+      </c>
+    </row>
+    <row r="2974" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2974" s="2" t="s">
+        <v>4013</v>
+      </c>
+      <c r="B2974" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C2974" s="2" t="s">
+        <v>4014</v>
+      </c>
+    </row>
+    <row r="2975" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2975" s="2" t="s">
+        <v>4015</v>
+      </c>
+      <c r="B2975" s="1">
+        <v>7.59</v>
+      </c>
+      <c r="C2975" s="2" t="s">
+        <v>3186</v>
+      </c>
+    </row>
+    <row r="2976" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2976" s="2" t="s">
+        <v>4016</v>
+      </c>
+      <c r="B2976" s="1">
+        <v>4.28</v>
+      </c>
+      <c r="C2976" s="2" t="s">
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="2977" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2977" s="2" t="s">
+        <v>4018</v>
+      </c>
+      <c r="B2977" s="1">
+        <v>6.15</v>
+      </c>
+      <c r="C2977" s="2" t="s">
+        <v>4019</v>
+      </c>
+    </row>
+    <row r="2978" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2978" s="2" t="s">
+        <v>4020</v>
+      </c>
+      <c r="B2978" s="1">
+        <v>6.43</v>
+      </c>
+      <c r="C2978" s="2" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="2979" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2979" s="2" t="s">
+        <v>4021</v>
+      </c>
+      <c r="B2979" s="1">
+        <v>8.19</v>
+      </c>
+      <c r="C2979" s="2" t="s">
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="2980" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2980" s="2" t="s">
+        <v>4023</v>
+      </c>
+      <c r="B2980" s="1">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="C2980" s="2" t="s">
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="2981" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2981" s="2" t="s">
+        <v>4025</v>
+      </c>
+      <c r="B2981" s="1">
+        <v>9.15</v>
+      </c>
+      <c r="C2981" s="2" t="s">
+        <v>4026</v>
+      </c>
+    </row>
+    <row r="2982" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2982" s="2" t="s">
+        <v>4027</v>
+      </c>
+      <c r="B2982" s="1">
+        <v>6.65</v>
+      </c>
+      <c r="C2982" s="2" t="s">
+        <v>4028</v>
+      </c>
+    </row>
+    <row r="2983" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2983" s="2" t="s">
+        <v>4029</v>
+      </c>
+      <c r="B2983" s="1">
+        <v>7.04</v>
+      </c>
+      <c r="C2983" s="2" t="s">
+        <v>3215</v>
+      </c>
+    </row>
+    <row r="2984" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2984" s="2" t="s">
+        <v>4030</v>
+      </c>
+      <c r="B2984" s="1">
+        <v>6.61</v>
+      </c>
+      <c r="C2984" s="2" t="s">
+        <v>4031</v>
+      </c>
+    </row>
+    <row r="2985" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2985" s="2" t="s">
+        <v>4032</v>
+      </c>
+      <c r="B2985" s="1">
+        <v>7.8</v>
+      </c>
+      <c r="C2985" s="2" t="s">
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="2986" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2986" s="2" t="s">
+        <v>4033</v>
+      </c>
+      <c r="B2986" s="1">
+        <v>5.66</v>
+      </c>
+      <c r="C2986" s="2" t="s">
+        <v>4034</v>
+      </c>
+    </row>
+    <row r="2987" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2987" s="2" t="s">
+        <v>4035</v>
+      </c>
+      <c r="B2987" s="1">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="C2987" s="2" t="s">
+        <v>2393</v>
+      </c>
+    </row>
+    <row r="2988" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2988" s="2" t="s">
+        <v>4036</v>
+      </c>
+      <c r="B2988" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="C2988" s="2" t="s">
+        <v>3454</v>
+      </c>
+    </row>
+    <row r="2989" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2989" s="2" t="s">
+        <v>4037</v>
+      </c>
+      <c r="B2989" s="1">
+        <v>8.93</v>
+      </c>
+      <c r="C2989" s="2" t="s">
+        <v>4038</v>
+      </c>
+    </row>
+    <row r="2990" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2990" s="2" t="s">
+        <v>4039</v>
+      </c>
+      <c r="B2990" s="1">
+        <v>4.42</v>
+      </c>
+      <c r="C2990" s="2" t="s">
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="2991" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2991" s="2" t="s">
+        <v>4041</v>
+      </c>
+      <c r="B2991" s="1">
+        <v>5.71</v>
+      </c>
+      <c r="C2991" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2992" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2992" s="2" t="s">
+        <v>4042</v>
+      </c>
+      <c r="B2992" s="1">
+        <v>7.35</v>
+      </c>
+      <c r="C2992" s="2" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="2993" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2993" s="2" t="s">
+        <v>4043</v>
+      </c>
+      <c r="B2993" s="1">
+        <v>9.26</v>
+      </c>
+      <c r="C2993" s="2" t="s">
+        <v>4044</v>
+      </c>
+    </row>
+    <row r="2994" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2994" s="2" t="s">
+        <v>4045</v>
+      </c>
+      <c r="B2994" s="1">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="C2994" s="2" t="s">
+        <v>4046</v>
+      </c>
+    </row>
+    <row r="2995" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2995" s="2" t="s">
+        <v>4047</v>
+      </c>
+      <c r="B2995" s="1">
+        <v>6.55</v>
+      </c>
+      <c r="C2995" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="2996" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2996" s="2" t="s">
+        <v>4048</v>
+      </c>
+      <c r="B2996" s="1">
+        <v>7</v>
+      </c>
+      <c r="C2996" s="2" t="s">
+        <v>4049</v>
+      </c>
+    </row>
+    <row r="2997" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2997" s="2" t="s">
+        <v>4050</v>
+      </c>
+      <c r="B2997" s="1">
+        <v>11.11</v>
+      </c>
+      <c r="C2997" s="2" t="s">
+        <v>4051</v>
+      </c>
+    </row>
+    <row r="2998" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2998" s="2" t="s">
+        <v>4052</v>
+      </c>
+      <c r="B2998" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="C2998" s="2" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="2999" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2999" s="2" t="s">
+        <v>4053</v>
+      </c>
+      <c r="B2999" s="1">
+        <v>4.24</v>
+      </c>
+      <c r="C2999" s="2" t="s">
+        <v>4054</v>
+      </c>
+    </row>
+    <row r="3000" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3000" s="2" t="s">
+        <v>4055</v>
+      </c>
+      <c r="B3000" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3000" s="2" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="3001" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3001" s="2" t="s">
+        <v>4057</v>
+      </c>
+      <c r="B3001" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="C3001" s="2" t="s">
+        <v>4058</v>
+      </c>
+    </row>
+    <row r="3002" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3002" s="2" t="s">
+        <v>4059</v>
+      </c>
+      <c r="B3002" s="1">
+        <v>12.08</v>
+      </c>
+      <c r="C3002" s="2" t="s">
+        <v>4060</v>
+      </c>
+    </row>
+    <row r="3003" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3003" s="2" t="s">
+        <v>4061</v>
+      </c>
+      <c r="B3003" s="1">
+        <v>6.23</v>
+      </c>
+      <c r="C3003" s="2" t="s">
+        <v>3503</v>
+      </c>
+    </row>
+    <row r="3004" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3004" s="2" t="s">
+        <v>4062</v>
+      </c>
+      <c r="B3004" s="1">
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="C3004" s="2" t="s">
+        <v>4063</v>
+      </c>
+    </row>
+    <row r="3005" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3005" s="2" t="s">
+        <v>4064</v>
+      </c>
+      <c r="B3005" s="1">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="C3005" s="2" t="s">
+        <v>4065</v>
+      </c>
+    </row>
+    <row r="3006" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3006" s="2" t="s">
+        <v>4066</v>
+      </c>
+      <c r="B3006" s="1">
+        <v>10.02</v>
+      </c>
+      <c r="C3006" s="2" t="s">
+        <v>4067</v>
+      </c>
+    </row>
+    <row r="3007" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3007" s="2" t="s">
+        <v>4068</v>
+      </c>
+      <c r="B3007" s="1">
+        <v>6.07</v>
+      </c>
+      <c r="C3007" s="2" t="s">
+        <v>4069</v>
+      </c>
+    </row>
+    <row r="3008" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3008" s="2" t="s">
+        <v>4070</v>
+      </c>
+      <c r="B3008" s="1">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="C3008" s="2" t="s">
+        <v>4071</v>
+      </c>
+    </row>
+    <row r="3009" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3009" s="2" t="s">
+        <v>4072</v>
+      </c>
+      <c r="B3009" s="1">
+        <v>8.23</v>
+      </c>
+      <c r="C3009" s="2" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="3010" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3010" s="2" t="s">
+        <v>4073</v>
+      </c>
+      <c r="B3010" s="1">
+        <v>11.67</v>
+      </c>
+      <c r="C3010" s="2" t="s">
+        <v>4074</v>
+      </c>
+    </row>
+    <row r="3011" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3011" s="2" t="s">
+        <v>4075</v>
+      </c>
+      <c r="B3011" s="1">
+        <v>8.18</v>
+      </c>
+      <c r="C3011" s="2" t="s">
+        <v>4076</v>
+      </c>
+    </row>
+    <row r="3012" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3012" s="2" t="s">
+        <v>4077</v>
+      </c>
+      <c r="B3012" s="1">
+        <v>8.35</v>
+      </c>
+      <c r="C3012" s="2" t="s">
+        <v>4078</v>
+      </c>
+    </row>
+    <row r="3013" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3013" s="2" t="s">
+        <v>4079</v>
+      </c>
+      <c r="B3013" s="1">
+        <v>9.11</v>
+      </c>
+      <c r="C3013" s="2" t="s">
+        <v>2370</v>
+      </c>
+    </row>
+    <row r="3014" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3014" s="2" t="s">
+        <v>4080</v>
+      </c>
+      <c r="B3014" s="1">
+        <v>12.11</v>
+      </c>
+      <c r="C3014" s="2" t="s">
+        <v>4081</v>
+      </c>
+    </row>
+    <row r="3015" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3015" s="2" t="s">
+        <v>4082</v>
+      </c>
+      <c r="B3015" s="1">
+        <v>5.01</v>
+      </c>
+      <c r="C3015" s="2" t="s">
+        <v>4083</v>
+      </c>
+    </row>
+    <row r="3016" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3016" s="2" t="s">
+        <v>4084</v>
+      </c>
+      <c r="B3016" s="1">
+        <v>6.29</v>
+      </c>
+      <c r="C3016" s="2" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="3017" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3017" s="2" t="s">
+        <v>4085</v>
+      </c>
+      <c r="B3017" s="1">
+        <v>3.11</v>
+      </c>
+      <c r="C3017" s="2" t="s">
+        <v>4086</v>
+      </c>
+    </row>
+    <row r="3018" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3018" s="2" t="s">
+        <v>4085</v>
+      </c>
+      <c r="B3018" s="1">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="3019" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3019" s="2" t="s">
+        <v>4087</v>
+      </c>
+      <c r="B3019" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="C3019" s="2" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3020" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3020" s="2" t="s">
+        <v>4088</v>
+      </c>
+      <c r="B3020" s="1">
+        <v>6.91</v>
+      </c>
+      <c r="C3020" s="2" t="s">
+        <v>4089</v>
+      </c>
+    </row>
+    <row r="3021" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3021" s="2" t="s">
+        <v>4090</v>
+      </c>
+      <c r="B3021" s="1">
+        <v>3.32</v>
+      </c>
+      <c r="C3021" s="2" t="s">
+        <v>2863</v>
+      </c>
+    </row>
+    <row r="3022" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3022" s="2" t="s">
+        <v>4090</v>
+      </c>
+      <c r="B3022" s="1">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="3023" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3023" s="2" t="s">
+        <v>4091</v>
+      </c>
+      <c r="B3023" s="1">
+        <v>6.22</v>
+      </c>
+      <c r="C3023" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3024" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3024" s="2" t="s">
+        <v>4092</v>
+      </c>
+      <c r="B3024" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3024" s="2" t="s">
+        <v>1927</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>